<commit_message>
fix(populate company and companyname from apollo source as well as its needed for mautic)
</commit_message>
<xml_diff>
--- a/output/merged_profiles_mautic.xlsx
+++ b/output/merged_profiles_mautic.xlsx
@@ -18110,7 +18110,11 @@
           <t>Wollsdorf Leather</t>
         </is>
       </c>
-      <c r="R190" t="inlineStr"/>
+      <c r="R190" t="inlineStr">
+        <is>
+          <t>Wollsdorf Leather</t>
+        </is>
+      </c>
       <c r="S190" t="inlineStr">
         <is>
           <t>140</t>
@@ -18197,7 +18201,11 @@
           <t>Rohrer Group</t>
         </is>
       </c>
-      <c r="R191" t="inlineStr"/>
+      <c r="R191" t="inlineStr">
+        <is>
+          <t>Rohrer Group</t>
+        </is>
+      </c>
       <c r="S191" t="inlineStr">
         <is>
           <t>270</t>
@@ -18276,7 +18284,11 @@
           <t>SGS Industrial Services GmbH</t>
         </is>
       </c>
-      <c r="R192" t="inlineStr"/>
+      <c r="R192" t="inlineStr">
+        <is>
+          <t>SGS Industrial Services GmbH</t>
+        </is>
+      </c>
       <c r="S192" t="inlineStr">
         <is>
           <t>120</t>
@@ -18355,7 +18367,11 @@
           <t>SIGMATEK Automation</t>
         </is>
       </c>
-      <c r="R193" t="inlineStr"/>
+      <c r="R193" t="inlineStr">
+        <is>
+          <t>SIGMATEK Automation</t>
+        </is>
+      </c>
       <c r="S193" t="inlineStr">
         <is>
           <t>160</t>
@@ -18446,7 +18462,11 @@
           <t>S.I.E</t>
         </is>
       </c>
-      <c r="R194" t="inlineStr"/>
+      <c r="R194" t="inlineStr">
+        <is>
+          <t>S.I.E</t>
+        </is>
+      </c>
       <c r="S194" t="inlineStr">
         <is>
           <t>72</t>
@@ -18529,7 +18549,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R195" t="inlineStr"/>
+      <c r="R195" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S195" t="inlineStr">
         <is>
           <t>49</t>
@@ -18612,7 +18636,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R196" t="inlineStr"/>
+      <c r="R196" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S196" t="inlineStr">
         <is>
           <t>49</t>
@@ -18691,7 +18719,11 @@
           <t>LTW Intralogistics GmbH</t>
         </is>
       </c>
-      <c r="R197" t="inlineStr"/>
+      <c r="R197" t="inlineStr">
+        <is>
+          <t>LTW Intralogistics GmbH</t>
+        </is>
+      </c>
       <c r="S197" t="inlineStr">
         <is>
           <t>200</t>
@@ -18774,7 +18806,11 @@
           <t>Porsche Wien</t>
         </is>
       </c>
-      <c r="R198" t="inlineStr"/>
+      <c r="R198" t="inlineStr">
+        <is>
+          <t>Porsche Wien</t>
+        </is>
+      </c>
       <c r="S198" t="inlineStr">
         <is>
           <t>65</t>
@@ -18857,7 +18893,11 @@
           <t>Schlumberger Wein- und Sektkellerei GmbH</t>
         </is>
       </c>
-      <c r="R199" t="inlineStr"/>
+      <c r="R199" t="inlineStr">
+        <is>
+          <t>Schlumberger Wein- und Sektkellerei GmbH</t>
+        </is>
+      </c>
       <c r="S199" t="inlineStr">
         <is>
           <t>56</t>
@@ -18948,7 +18988,11 @@
           <t>ERGO Austria</t>
         </is>
       </c>
-      <c r="R200" t="inlineStr"/>
+      <c r="R200" t="inlineStr">
+        <is>
+          <t>ERGO Austria</t>
+        </is>
+      </c>
       <c r="S200" t="inlineStr">
         <is>
           <t>230</t>
@@ -19031,7 +19075,11 @@
           <t>Berger Logistik</t>
         </is>
       </c>
-      <c r="R201" t="inlineStr"/>
+      <c r="R201" t="inlineStr">
+        <is>
+          <t>Berger Logistik</t>
+        </is>
+      </c>
       <c r="S201" t="inlineStr">
         <is>
           <t>110</t>
@@ -19110,7 +19158,11 @@
           <t>Planquadr.at</t>
         </is>
       </c>
-      <c r="R202" t="inlineStr"/>
+      <c r="R202" t="inlineStr">
+        <is>
+          <t>Planquadr.at</t>
+        </is>
+      </c>
       <c r="S202" t="inlineStr">
         <is>
           <t>16</t>
@@ -19193,7 +19245,11 @@
           <t>Doppelmayr Official</t>
         </is>
       </c>
-      <c r="R203" t="inlineStr"/>
+      <c r="R203" t="inlineStr">
+        <is>
+          <t>Doppelmayr Official</t>
+        </is>
+      </c>
       <c r="S203" t="inlineStr">
         <is>
           <t>420</t>
@@ -19280,7 +19336,11 @@
           <t>VFI GmbH</t>
         </is>
       </c>
-      <c r="R204" t="inlineStr"/>
+      <c r="R204" t="inlineStr">
+        <is>
+          <t>VFI GmbH</t>
+        </is>
+      </c>
       <c r="S204" t="inlineStr">
         <is>
           <t>75</t>
@@ -19359,7 +19419,11 @@
           <t>Gföllner Fahrzeugbau und Containertechnik GmbH</t>
         </is>
       </c>
-      <c r="R205" t="inlineStr"/>
+      <c r="R205" t="inlineStr">
+        <is>
+          <t>Gföllner Fahrzeugbau und Containertechnik GmbH</t>
+        </is>
+      </c>
       <c r="S205" t="inlineStr">
         <is>
           <t>56</t>
@@ -19450,7 +19514,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R206" t="inlineStr"/>
+      <c r="R206" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S206" t="inlineStr">
         <is>
           <t>49</t>
@@ -19525,7 +19593,11 @@
           <t>AustroCel Hallein GmbH</t>
         </is>
       </c>
-      <c r="R207" t="inlineStr"/>
+      <c r="R207" t="inlineStr">
+        <is>
+          <t>AustroCel Hallein GmbH</t>
+        </is>
+      </c>
       <c r="S207" t="inlineStr">
         <is>
           <t>83</t>
@@ -19608,7 +19680,11 @@
           <t>Greiner Assistec</t>
         </is>
       </c>
-      <c r="R208" t="inlineStr"/>
+      <c r="R208" t="inlineStr">
+        <is>
+          <t>Greiner Assistec</t>
+        </is>
+      </c>
       <c r="S208" t="inlineStr">
         <is>
           <t>220</t>
@@ -19687,7 +19763,11 @@
           <t>Global Hydro Energy</t>
         </is>
       </c>
-      <c r="R209" t="inlineStr"/>
+      <c r="R209" t="inlineStr">
+        <is>
+          <t>Global Hydro Energy</t>
+        </is>
+      </c>
       <c r="S209" t="inlineStr">
         <is>
           <t>220</t>
@@ -19770,7 +19850,11 @@
           <t>AVUS</t>
         </is>
       </c>
-      <c r="R210" t="inlineStr"/>
+      <c r="R210" t="inlineStr">
+        <is>
+          <t>AVUS</t>
+        </is>
+      </c>
       <c r="S210" t="inlineStr">
         <is>
           <t>92</t>
@@ -19853,7 +19937,11 @@
           <t>Alpine Metal Tech Group</t>
         </is>
       </c>
-      <c r="R211" t="inlineStr"/>
+      <c r="R211" t="inlineStr">
+        <is>
+          <t>Alpine Metal Tech Group</t>
+        </is>
+      </c>
       <c r="S211" t="inlineStr">
         <is>
           <t>170</t>
@@ -19944,7 +20032,11 @@
           <t>Lexogen</t>
         </is>
       </c>
-      <c r="R212" t="inlineStr"/>
+      <c r="R212" t="inlineStr">
+        <is>
+          <t>Lexogen</t>
+        </is>
+      </c>
       <c r="S212" t="inlineStr">
         <is>
           <t>79</t>
@@ -20027,7 +20119,11 @@
           <t>UIV Urban Innovation Vienna</t>
         </is>
       </c>
-      <c r="R213" t="inlineStr"/>
+      <c r="R213" t="inlineStr">
+        <is>
+          <t>UIV Urban Innovation Vienna</t>
+        </is>
+      </c>
       <c r="S213" t="inlineStr">
         <is>
           <t>65</t>
@@ -20110,7 +20206,11 @@
           <t>Instahelp</t>
         </is>
       </c>
-      <c r="R214" t="inlineStr"/>
+      <c r="R214" t="inlineStr">
+        <is>
+          <t>Instahelp</t>
+        </is>
+      </c>
       <c r="S214" t="inlineStr">
         <is>
           <t>100</t>
@@ -20201,7 +20301,11 @@
           <t>Tyromotion</t>
         </is>
       </c>
-      <c r="R215" t="inlineStr"/>
+      <c r="R215" t="inlineStr">
+        <is>
+          <t>Tyromotion</t>
+        </is>
+      </c>
       <c r="S215" t="inlineStr">
         <is>
           <t>72</t>
@@ -20288,7 +20392,11 @@
           <t>AMEX Healthcare</t>
         </is>
       </c>
-      <c r="R216" t="inlineStr"/>
+      <c r="R216" t="inlineStr">
+        <is>
+          <t>AMEX Healthcare</t>
+        </is>
+      </c>
       <c r="S216" t="inlineStr">
         <is>
           <t>290</t>
@@ -20367,7 +20475,11 @@
           <t>Krankenhaus der Elisabethinen</t>
         </is>
       </c>
-      <c r="R217" t="inlineStr"/>
+      <c r="R217" t="inlineStr">
+        <is>
+          <t>Krankenhaus der Elisabethinen</t>
+        </is>
+      </c>
       <c r="S217" t="inlineStr">
         <is>
           <t>120</t>
@@ -20454,7 +20566,11 @@
           <t>Croma-Pharma</t>
         </is>
       </c>
-      <c r="R218" t="inlineStr"/>
+      <c r="R218" t="inlineStr">
+        <is>
+          <t>Croma-Pharma</t>
+        </is>
+      </c>
       <c r="S218" t="inlineStr">
         <is>
           <t>470</t>
@@ -20545,7 +20661,11 @@
           <t>StartUs Insights</t>
         </is>
       </c>
-      <c r="R219" t="inlineStr"/>
+      <c r="R219" t="inlineStr">
+        <is>
+          <t>StartUs Insights</t>
+        </is>
+      </c>
       <c r="S219" t="inlineStr">
         <is>
           <t>52</t>
@@ -20628,7 +20748,11 @@
           <t>SynthesaGruppe</t>
         </is>
       </c>
-      <c r="R220" t="inlineStr"/>
+      <c r="R220" t="inlineStr">
+        <is>
+          <t>SynthesaGruppe</t>
+        </is>
+      </c>
       <c r="S220" t="inlineStr">
         <is>
           <t>160</t>
@@ -20719,7 +20843,11 @@
           <t>CCE</t>
         </is>
       </c>
-      <c r="R221" t="inlineStr"/>
+      <c r="R221" t="inlineStr">
+        <is>
+          <t>CCE</t>
+        </is>
+      </c>
       <c r="S221" t="inlineStr">
         <is>
           <t>310</t>
@@ -20794,7 +20922,11 @@
           <t>Croma-Pharma</t>
         </is>
       </c>
-      <c r="R222" t="inlineStr"/>
+      <c r="R222" t="inlineStr">
+        <is>
+          <t>Croma-Pharma</t>
+        </is>
+      </c>
       <c r="S222" t="inlineStr">
         <is>
           <t>470</t>
@@ -20881,7 +21013,11 @@
           <t>AGILOX</t>
         </is>
       </c>
-      <c r="R223" t="inlineStr"/>
+      <c r="R223" t="inlineStr">
+        <is>
+          <t>AGILOX</t>
+        </is>
+      </c>
       <c r="S223" t="inlineStr">
         <is>
           <t>170</t>
@@ -20968,7 +21104,11 @@
           <t>myflexbox</t>
         </is>
       </c>
-      <c r="R224" t="inlineStr"/>
+      <c r="R224" t="inlineStr">
+        <is>
+          <t>myflexbox</t>
+        </is>
+      </c>
       <c r="S224" t="inlineStr">
         <is>
           <t>63</t>
@@ -21051,7 +21191,11 @@
           <t>TAG GmbH</t>
         </is>
       </c>
-      <c r="R225" t="inlineStr"/>
+      <c r="R225" t="inlineStr">
+        <is>
+          <t>TAG GmbH</t>
+        </is>
+      </c>
       <c r="S225" t="inlineStr">
         <is>
           <t>110</t>
@@ -21130,7 +21274,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R226" t="inlineStr"/>
+      <c r="R226" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S226" t="inlineStr">
         <is>
           <t>410</t>
@@ -21209,7 +21357,11 @@
           <t>viadonau</t>
         </is>
       </c>
-      <c r="R227" t="inlineStr"/>
+      <c r="R227" t="inlineStr">
+        <is>
+          <t>viadonau</t>
+        </is>
+      </c>
       <c r="S227" t="inlineStr">
         <is>
           <t>98</t>
@@ -21296,7 +21448,11 @@
           <t>Trotec Laser</t>
         </is>
       </c>
-      <c r="R228" t="inlineStr"/>
+      <c r="R228" t="inlineStr">
+        <is>
+          <t>Trotec Laser</t>
+        </is>
+      </c>
       <c r="S228" t="inlineStr">
         <is>
           <t>390</t>
@@ -21387,7 +21543,11 @@
           <t>A.M.I. Agency for Medical Innovations GmbH</t>
         </is>
       </c>
-      <c r="R229" t="inlineStr"/>
+      <c r="R229" t="inlineStr">
+        <is>
+          <t>A.M.I. Agency for Medical Innovations GmbH</t>
+        </is>
+      </c>
       <c r="S229" t="inlineStr">
         <is>
           <t>63</t>
@@ -21478,7 +21638,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R230" t="inlineStr"/>
+      <c r="R230" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S230" t="inlineStr">
         <is>
           <t>49</t>
@@ -21569,7 +21733,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R231" t="inlineStr"/>
+      <c r="R231" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S231" t="inlineStr">
         <is>
           <t>49</t>
@@ -21660,7 +21828,11 @@
           <t>AustroCel Hallein GmbH</t>
         </is>
       </c>
-      <c r="R232" t="inlineStr"/>
+      <c r="R232" t="inlineStr">
+        <is>
+          <t>AustroCel Hallein GmbH</t>
+        </is>
+      </c>
       <c r="S232" t="inlineStr">
         <is>
           <t>81</t>
@@ -21751,7 +21923,11 @@
           <t>KOBAN SÜDVERS</t>
         </is>
       </c>
-      <c r="R233" t="inlineStr"/>
+      <c r="R233" t="inlineStr">
+        <is>
+          <t>KOBAN SÜDVERS</t>
+        </is>
+      </c>
       <c r="S233" t="inlineStr">
         <is>
           <t>50</t>
@@ -21838,7 +22014,11 @@
           <t>RAG Austria AG</t>
         </is>
       </c>
-      <c r="R234" t="inlineStr"/>
+      <c r="R234" t="inlineStr">
+        <is>
+          <t>RAG Austria AG</t>
+        </is>
+      </c>
       <c r="S234" t="inlineStr">
         <is>
           <t>170</t>
@@ -21925,7 +22105,11 @@
           <t>European Academy of Neurology</t>
         </is>
       </c>
-      <c r="R235" t="inlineStr"/>
+      <c r="R235" t="inlineStr">
+        <is>
+          <t>European Academy of Neurology</t>
+        </is>
+      </c>
       <c r="S235" t="inlineStr">
         <is>
           <t>270</t>
@@ -22012,7 +22196,11 @@
           <t>Binder+Co AG</t>
         </is>
       </c>
-      <c r="R236" t="inlineStr"/>
+      <c r="R236" t="inlineStr">
+        <is>
+          <t>Binder+Co AG</t>
+        </is>
+      </c>
       <c r="S236" t="inlineStr">
         <is>
           <t>110</t>
@@ -22099,7 +22287,11 @@
           <t>pharma&amp;</t>
         </is>
       </c>
-      <c r="R237" t="inlineStr"/>
+      <c r="R237" t="inlineStr">
+        <is>
+          <t>pharma&amp;</t>
+        </is>
+      </c>
       <c r="S237" t="inlineStr">
         <is>
           <t>150</t>
@@ -22190,7 +22382,11 @@
           <t>enspired</t>
         </is>
       </c>
-      <c r="R238" t="inlineStr"/>
+      <c r="R238" t="inlineStr">
+        <is>
+          <t>enspired</t>
+        </is>
+      </c>
       <c r="S238" t="inlineStr">
         <is>
           <t>85</t>
@@ -22277,7 +22473,11 @@
           <t>Federal Ministry of Labour and Economy</t>
         </is>
       </c>
-      <c r="R239" t="inlineStr"/>
+      <c r="R239" t="inlineStr">
+        <is>
+          <t>Federal Ministry of Labour and Economy</t>
+        </is>
+      </c>
       <c r="S239" t="inlineStr">
         <is>
           <t>480</t>
@@ -22360,7 +22560,11 @@
           <t>Die eww Gruppe</t>
         </is>
       </c>
-      <c r="R240" t="inlineStr"/>
+      <c r="R240" t="inlineStr">
+        <is>
+          <t>Die eww Gruppe</t>
+        </is>
+      </c>
       <c r="S240" t="inlineStr">
         <is>
           <t>250</t>
@@ -22443,7 +22647,11 @@
           <t>EBNER GROUP</t>
         </is>
       </c>
-      <c r="R241" t="inlineStr"/>
+      <c r="R241" t="inlineStr">
+        <is>
+          <t>EBNER GROUP</t>
+        </is>
+      </c>
       <c r="S241" t="inlineStr">
         <is>
           <t>48</t>
@@ -22530,7 +22738,11 @@
           <t>ISOVOLTA Group</t>
         </is>
       </c>
-      <c r="R242" t="inlineStr"/>
+      <c r="R242" t="inlineStr">
+        <is>
+          <t>ISOVOLTA Group</t>
+        </is>
+      </c>
       <c r="S242" t="inlineStr">
         <is>
           <t>440</t>
@@ -22617,7 +22829,11 @@
           <t>Alpine Metal Tech Group</t>
         </is>
       </c>
-      <c r="R243" t="inlineStr"/>
+      <c r="R243" t="inlineStr">
+        <is>
+          <t>Alpine Metal Tech Group</t>
+        </is>
+      </c>
       <c r="S243" t="inlineStr">
         <is>
           <t>160</t>
@@ -22704,7 +22920,11 @@
           <t>AUSTRIA JUICE Group</t>
         </is>
       </c>
-      <c r="R244" t="inlineStr"/>
+      <c r="R244" t="inlineStr">
+        <is>
+          <t>AUSTRIA JUICE Group</t>
+        </is>
+      </c>
       <c r="S244" t="inlineStr">
         <is>
           <t>160</t>
@@ -22791,7 +23011,11 @@
           <t>POLOPLAST GmbH &amp; Co KG</t>
         </is>
       </c>
-      <c r="R245" t="inlineStr"/>
+      <c r="R245" t="inlineStr">
+        <is>
+          <t>POLOPLAST GmbH &amp; Co KG</t>
+        </is>
+      </c>
       <c r="S245" t="inlineStr">
         <is>
           <t>140</t>
@@ -22870,7 +23094,11 @@
           <t>Winkelbauer</t>
         </is>
       </c>
-      <c r="R246" t="inlineStr"/>
+      <c r="R246" t="inlineStr">
+        <is>
+          <t>Winkelbauer</t>
+        </is>
+      </c>
       <c r="S246" t="inlineStr">
         <is>
           <t>52</t>
@@ -22957,7 +23185,11 @@
           <t>Lagermax Group</t>
         </is>
       </c>
-      <c r="R247" t="inlineStr"/>
+      <c r="R247" t="inlineStr">
+        <is>
+          <t>Lagermax Group</t>
+        </is>
+      </c>
       <c r="S247" t="inlineStr">
         <is>
           <t>340</t>
@@ -23032,7 +23264,11 @@
           <t>Amt der Salzburger Landesregierung</t>
         </is>
       </c>
-      <c r="R248" t="inlineStr"/>
+      <c r="R248" t="inlineStr">
+        <is>
+          <t>Amt der Salzburger Landesregierung</t>
+        </is>
+      </c>
       <c r="S248" t="inlineStr">
         <is>
           <t>340</t>
@@ -23119,7 +23355,11 @@
           <t>Wiener Privatklinik</t>
         </is>
       </c>
-      <c r="R249" t="inlineStr"/>
+      <c r="R249" t="inlineStr">
+        <is>
+          <t>Wiener Privatklinik</t>
+        </is>
+      </c>
       <c r="S249" t="inlineStr">
         <is>
           <t>85</t>
@@ -23198,7 +23438,11 @@
           <t>Carinthian State Insurance Company</t>
         </is>
       </c>
-      <c r="R250" t="inlineStr"/>
+      <c r="R250" t="inlineStr">
+        <is>
+          <t>Carinthian State Insurance Company</t>
+        </is>
+      </c>
       <c r="S250" t="inlineStr">
         <is>
           <t>56</t>
@@ -23285,7 +23529,11 @@
           <t>VEGA International Car-Transport and Logistic-Trading GmbH</t>
         </is>
       </c>
-      <c r="R251" t="inlineStr"/>
+      <c r="R251" t="inlineStr">
+        <is>
+          <t>VEGA International Car-Transport and Logistic-Trading GmbH</t>
+        </is>
+      </c>
       <c r="S251" t="inlineStr">
         <is>
           <t>51</t>
@@ -23360,7 +23608,11 @@
           <t>Die eww Gruppe</t>
         </is>
       </c>
-      <c r="R252" t="inlineStr"/>
+      <c r="R252" t="inlineStr">
+        <is>
+          <t>Die eww Gruppe</t>
+        </is>
+      </c>
       <c r="S252" t="inlineStr">
         <is>
           <t>250</t>
@@ -23447,7 +23699,11 @@
           <t>VFI GmbH</t>
         </is>
       </c>
-      <c r="R253" t="inlineStr"/>
+      <c r="R253" t="inlineStr">
+        <is>
+          <t>VFI GmbH</t>
+        </is>
+      </c>
       <c r="S253" t="inlineStr">
         <is>
           <t>75</t>
@@ -23534,7 +23790,11 @@
           <t>Fraunhofer Austria</t>
         </is>
       </c>
-      <c r="R254" t="inlineStr"/>
+      <c r="R254" t="inlineStr">
+        <is>
+          <t>Fraunhofer Austria</t>
+        </is>
+      </c>
       <c r="S254" t="inlineStr">
         <is>
           <t>130</t>
@@ -23617,7 +23877,11 @@
           <t>byrd</t>
         </is>
       </c>
-      <c r="R255" t="inlineStr"/>
+      <c r="R255" t="inlineStr">
+        <is>
+          <t>byrd</t>
+        </is>
+      </c>
       <c r="S255" t="inlineStr">
         <is>
           <t>170</t>
@@ -23700,7 +23964,11 @@
           <t>Storebox</t>
         </is>
       </c>
-      <c r="R256" t="inlineStr"/>
+      <c r="R256" t="inlineStr">
+        <is>
+          <t>Storebox</t>
+        </is>
+      </c>
       <c r="S256" t="inlineStr">
         <is>
           <t>100</t>
@@ -23775,7 +24043,11 @@
           <t>Stadtwerke Klagenfurt AG</t>
         </is>
       </c>
-      <c r="R257" t="inlineStr"/>
+      <c r="R257" t="inlineStr">
+        <is>
+          <t>Stadtwerke Klagenfurt AG</t>
+        </is>
+      </c>
       <c r="S257" t="inlineStr">
         <is>
           <t>150</t>
@@ -23858,7 +24130,11 @@
           <t>Novogenia GmbH</t>
         </is>
       </c>
-      <c r="R258" t="inlineStr"/>
+      <c r="R258" t="inlineStr">
+        <is>
+          <t>Novogenia GmbH</t>
+        </is>
+      </c>
       <c r="S258" t="inlineStr">
         <is>
           <t>74</t>
@@ -23941,7 +24217,11 @@
           <t>Weingärtner Maschinenbau GmbH</t>
         </is>
       </c>
-      <c r="R259" t="inlineStr"/>
+      <c r="R259" t="inlineStr">
+        <is>
+          <t>Weingärtner Maschinenbau GmbH</t>
+        </is>
+      </c>
       <c r="S259" t="inlineStr">
         <is>
           <t>62</t>
@@ -24016,7 +24296,11 @@
           <t>Häuser zum Leben</t>
         </is>
       </c>
-      <c r="R260" t="inlineStr"/>
+      <c r="R260" t="inlineStr">
+        <is>
+          <t>Häuser zum Leben</t>
+        </is>
+      </c>
       <c r="S260" t="inlineStr">
         <is>
           <t>420</t>
@@ -24099,7 +24383,11 @@
           <t>Tauernklinikum</t>
         </is>
       </c>
-      <c r="R261" t="inlineStr"/>
+      <c r="R261" t="inlineStr">
+        <is>
+          <t>Tauernklinikum</t>
+        </is>
+      </c>
       <c r="S261" t="inlineStr">
         <is>
           <t>110</t>
@@ -24174,7 +24462,11 @@
           <t>g.tec medical engineering GmbH - NEVER STOP RECORDING</t>
         </is>
       </c>
-      <c r="R262" t="inlineStr"/>
+      <c r="R262" t="inlineStr">
+        <is>
+          <t>g.tec medical engineering GmbH - NEVER STOP RECORDING</t>
+        </is>
+      </c>
       <c r="S262" t="inlineStr">
         <is>
           <t>65</t>
@@ -24257,7 +24549,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R263" t="inlineStr"/>
+      <c r="R263" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S263" t="inlineStr">
         <is>
           <t>400</t>
@@ -24340,7 +24636,11 @@
           <t>Hagleitner Hygiene International GmbH</t>
         </is>
       </c>
-      <c r="R264" t="inlineStr"/>
+      <c r="R264" t="inlineStr">
+        <is>
+          <t>Hagleitner Hygiene International GmbH</t>
+        </is>
+      </c>
       <c r="S264" t="inlineStr">
         <is>
           <t>490</t>
@@ -24415,7 +24715,11 @@
           <t>CS Caritas Socialis</t>
         </is>
       </c>
-      <c r="R265" t="inlineStr"/>
+      <c r="R265" t="inlineStr">
+        <is>
+          <t>CS Caritas Socialis</t>
+        </is>
+      </c>
       <c r="S265" t="inlineStr">
         <is>
           <t>120</t>
@@ -24498,7 +24802,11 @@
           <t>Psychosoziale Dienste in Wien</t>
         </is>
       </c>
-      <c r="R266" t="inlineStr"/>
+      <c r="R266" t="inlineStr">
+        <is>
+          <t>Psychosoziale Dienste in Wien</t>
+        </is>
+      </c>
       <c r="S266" t="inlineStr">
         <is>
           <t>71</t>
@@ -24581,7 +24889,11 @@
           <t>Energie Graz</t>
         </is>
       </c>
-      <c r="R267" t="inlineStr"/>
+      <c r="R267" t="inlineStr">
+        <is>
+          <t>Energie Graz</t>
+        </is>
+      </c>
       <c r="S267" t="inlineStr">
         <is>
           <t>120</t>
@@ -24660,7 +24972,11 @@
           <t>VOGL + CO</t>
         </is>
       </c>
-      <c r="R268" t="inlineStr"/>
+      <c r="R268" t="inlineStr">
+        <is>
+          <t>VOGL + CO</t>
+        </is>
+      </c>
       <c r="S268" t="inlineStr">
         <is>
           <t>60</t>
@@ -24743,7 +25059,11 @@
           <t>Röhren- und Pumpenwerk Bauer GmbH</t>
         </is>
       </c>
-      <c r="R269" t="inlineStr"/>
+      <c r="R269" t="inlineStr">
+        <is>
+          <t>Röhren- und Pumpenwerk Bauer GmbH</t>
+        </is>
+      </c>
       <c r="S269" t="inlineStr">
         <is>
           <t>54</t>
@@ -24822,7 +25142,11 @@
           <t>Hochreiter Fleischwaren GmbH</t>
         </is>
       </c>
-      <c r="R270" t="inlineStr"/>
+      <c r="R270" t="inlineStr">
+        <is>
+          <t>Hochreiter Fleischwaren GmbH</t>
+        </is>
+      </c>
       <c r="S270" t="inlineStr">
         <is>
           <t>51</t>
@@ -24901,7 +25225,11 @@
           <t>Häuser zum Leben</t>
         </is>
       </c>
-      <c r="R271" t="inlineStr"/>
+      <c r="R271" t="inlineStr">
+        <is>
+          <t>Häuser zum Leben</t>
+        </is>
+      </c>
       <c r="S271" t="inlineStr">
         <is>
           <t>420</t>
@@ -24976,7 +25304,11 @@
           <t>JOANNEUM RESEARCH</t>
         </is>
       </c>
-      <c r="R272" t="inlineStr"/>
+      <c r="R272" t="inlineStr">
+        <is>
+          <t>JOANNEUM RESEARCH</t>
+        </is>
+      </c>
       <c r="S272" t="inlineStr">
         <is>
           <t>390</t>
@@ -25059,7 +25391,11 @@
           <t>ENcome Energy Performance</t>
         </is>
       </c>
-      <c r="R273" t="inlineStr"/>
+      <c r="R273" t="inlineStr">
+        <is>
+          <t>ENcome Energy Performance</t>
+        </is>
+      </c>
       <c r="S273" t="inlineStr">
         <is>
           <t>85</t>
@@ -25142,7 +25478,11 @@
           <t>Ankerbrot</t>
         </is>
       </c>
-      <c r="R274" t="inlineStr"/>
+      <c r="R274" t="inlineStr">
+        <is>
+          <t>Ankerbrot</t>
+        </is>
+      </c>
       <c r="S274" t="inlineStr">
         <is>
           <t>130</t>
@@ -25217,7 +25557,11 @@
           <t>AMST-Systemtechnik GmbH</t>
         </is>
       </c>
-      <c r="R275" t="inlineStr"/>
+      <c r="R275" t="inlineStr">
+        <is>
+          <t>AMST-Systemtechnik GmbH</t>
+        </is>
+      </c>
       <c r="S275" t="inlineStr">
         <is>
           <t>85</t>
@@ -25300,7 +25644,11 @@
           <t>Sonnleitner GmbH</t>
         </is>
       </c>
-      <c r="R276" t="inlineStr"/>
+      <c r="R276" t="inlineStr">
+        <is>
+          <t>Sonnleitner GmbH</t>
+        </is>
+      </c>
       <c r="S276" t="inlineStr">
         <is>
           <t>110</t>
@@ -25375,7 +25723,11 @@
           <t>Oberoesterreichische Gebietskrankenkasse</t>
         </is>
       </c>
-      <c r="R277" t="inlineStr"/>
+      <c r="R277" t="inlineStr">
+        <is>
+          <t>Oberoesterreichische Gebietskrankenkasse</t>
+        </is>
+      </c>
       <c r="S277" t="inlineStr">
         <is>
           <t>63</t>
@@ -25446,7 +25798,11 @@
           <t>faigle Kunststoffe GmbH</t>
         </is>
       </c>
-      <c r="R278" t="inlineStr"/>
+      <c r="R278" t="inlineStr">
+        <is>
+          <t>faigle Kunststoffe GmbH</t>
+        </is>
+      </c>
       <c r="S278" t="inlineStr">
         <is>
           <t>64</t>
@@ -25521,7 +25877,11 @@
           <t>EFM Versicherungsmakler</t>
         </is>
       </c>
-      <c r="R279" t="inlineStr"/>
+      <c r="R279" t="inlineStr">
+        <is>
+          <t>EFM Versicherungsmakler</t>
+        </is>
+      </c>
       <c r="S279" t="inlineStr">
         <is>
           <t>67</t>
@@ -25600,7 +25960,11 @@
           <t>Pörner Ingenieurgesellschaft mbH</t>
         </is>
       </c>
-      <c r="R280" t="inlineStr"/>
+      <c r="R280" t="inlineStr">
+        <is>
+          <t>Pörner Ingenieurgesellschaft mbH</t>
+        </is>
+      </c>
       <c r="S280" t="inlineStr">
         <is>
           <t>140</t>
@@ -25683,7 +26047,11 @@
           <t>Lucky Car Austria</t>
         </is>
       </c>
-      <c r="R281" t="inlineStr"/>
+      <c r="R281" t="inlineStr">
+        <is>
+          <t>Lucky Car Austria</t>
+        </is>
+      </c>
       <c r="S281" t="inlineStr">
         <is>
           <t>58</t>
@@ -25766,7 +26134,11 @@
           <t>myflexbox</t>
         </is>
       </c>
-      <c r="R282" t="inlineStr"/>
+      <c r="R282" t="inlineStr">
+        <is>
+          <t>myflexbox</t>
+        </is>
+      </c>
       <c r="S282" t="inlineStr">
         <is>
           <t>62</t>
@@ -25841,7 +26213,11 @@
           <t>hollu Systemhygiene GmbH</t>
         </is>
       </c>
-      <c r="R283" t="inlineStr"/>
+      <c r="R283" t="inlineStr">
+        <is>
+          <t>hollu Systemhygiene GmbH</t>
+        </is>
+      </c>
       <c r="S283" t="inlineStr">
         <is>
           <t>210</t>
@@ -25920,7 +26296,11 @@
           <t>AGILOX</t>
         </is>
       </c>
-      <c r="R284" t="inlineStr"/>
+      <c r="R284" t="inlineStr">
+        <is>
+          <t>AGILOX</t>
+        </is>
+      </c>
       <c r="S284" t="inlineStr">
         <is>
           <t>180</t>
@@ -25995,7 +26375,11 @@
           <t>TROX Austria &amp; CEE</t>
         </is>
       </c>
-      <c r="R285" t="inlineStr"/>
+      <c r="R285" t="inlineStr">
+        <is>
+          <t>TROX Austria &amp; CEE</t>
+        </is>
+      </c>
       <c r="S285" t="inlineStr">
         <is>
           <t>51</t>
@@ -26070,7 +26454,11 @@
           <t>GIG Karasek GmbH - A Member of Dr. Aichhorn Group</t>
         </is>
       </c>
-      <c r="R286" t="inlineStr"/>
+      <c r="R286" t="inlineStr">
+        <is>
+          <t>GIG Karasek GmbH - A Member of Dr. Aichhorn Group</t>
+        </is>
+      </c>
       <c r="S286" t="inlineStr">
         <is>
           <t>68</t>
@@ -26153,7 +26541,11 @@
           <t>PremiQaMed Group</t>
         </is>
       </c>
-      <c r="R287" t="inlineStr"/>
+      <c r="R287" t="inlineStr">
+        <is>
+          <t>PremiQaMed Group</t>
+        </is>
+      </c>
       <c r="S287" t="inlineStr">
         <is>
           <t>380</t>
@@ -26236,7 +26628,11 @@
           <t>Lanserhof Group</t>
         </is>
       </c>
-      <c r="R288" t="inlineStr"/>
+      <c r="R288" t="inlineStr">
+        <is>
+          <t>Lanserhof Group</t>
+        </is>
+      </c>
       <c r="S288" t="inlineStr">
         <is>
           <t>160</t>
@@ -26319,7 +26715,11 @@
           <t>HAGE Sondermaschinenbau GmbH</t>
         </is>
       </c>
-      <c r="R289" t="inlineStr"/>
+      <c r="R289" t="inlineStr">
+        <is>
+          <t>HAGE Sondermaschinenbau GmbH</t>
+        </is>
+      </c>
       <c r="S289" t="inlineStr">
         <is>
           <t>51</t>
@@ -26395,7 +26795,11 @@
           <t>CS Caritas Socialis</t>
         </is>
       </c>
-      <c r="R290" t="inlineStr"/>
+      <c r="R290" t="inlineStr">
+        <is>
+          <t>CS Caritas Socialis</t>
+        </is>
+      </c>
       <c r="S290" t="inlineStr">
         <is>
           <t>120</t>
@@ -26478,7 +26882,11 @@
           <t>Austrian Federal Chancellery</t>
         </is>
       </c>
-      <c r="R291" t="inlineStr"/>
+      <c r="R291" t="inlineStr">
+        <is>
+          <t>Austrian Federal Chancellery</t>
+        </is>
+      </c>
       <c r="S291" t="inlineStr">
         <is>
           <t>86</t>
@@ -26553,7 +26961,11 @@
           <t>Hödlmayr International AG</t>
         </is>
       </c>
-      <c r="R292" t="inlineStr"/>
+      <c r="R292" t="inlineStr">
+        <is>
+          <t>Hödlmayr International AG</t>
+        </is>
+      </c>
       <c r="S292" t="inlineStr">
         <is>
           <t>280</t>
@@ -26628,7 +27040,11 @@
           <t>Kremsmueller</t>
         </is>
       </c>
-      <c r="R293" t="inlineStr"/>
+      <c r="R293" t="inlineStr">
+        <is>
+          <t>Kremsmueller</t>
+        </is>
+      </c>
       <c r="S293" t="inlineStr">
         <is>
           <t>310</t>
@@ -26711,7 +27127,11 @@
           <t>Barmherzige Schwestern Krankenhaus Wien</t>
         </is>
       </c>
-      <c r="R294" t="inlineStr"/>
+      <c r="R294" t="inlineStr">
+        <is>
+          <t>Barmherzige Schwestern Krankenhaus Wien</t>
+        </is>
+      </c>
       <c r="S294" t="inlineStr">
         <is>
           <t>170</t>
@@ -26786,7 +27206,11 @@
           <t>Neuroth</t>
         </is>
       </c>
-      <c r="R295" t="inlineStr"/>
+      <c r="R295" t="inlineStr">
+        <is>
+          <t>Neuroth</t>
+        </is>
+      </c>
       <c r="S295" t="inlineStr">
         <is>
           <t>420</t>
@@ -26869,7 +27293,11 @@
           <t>A. ö. Krankenhaus Spittal/Drau</t>
         </is>
       </c>
-      <c r="R296" t="inlineStr"/>
+      <c r="R296" t="inlineStr">
+        <is>
+          <t>A. ö. Krankenhaus Spittal/Drau</t>
+        </is>
+      </c>
       <c r="S296" t="inlineStr">
         <is>
           <t>57</t>
@@ -26952,7 +27380,11 @@
           <t>Lucky Car Austria</t>
         </is>
       </c>
-      <c r="R297" t="inlineStr"/>
+      <c r="R297" t="inlineStr">
+        <is>
+          <t>Lucky Car Austria</t>
+        </is>
+      </c>
       <c r="S297" t="inlineStr">
         <is>
           <t>58</t>
@@ -27027,7 +27459,11 @@
           <t>Federal Office of Metrology and Surveying (BEV)</t>
         </is>
       </c>
-      <c r="R298" t="inlineStr"/>
+      <c r="R298" t="inlineStr">
+        <is>
+          <t>Federal Office of Metrology and Surveying (BEV)</t>
+        </is>
+      </c>
       <c r="S298" t="inlineStr">
         <is>
           <t>160</t>
@@ -27102,7 +27538,11 @@
           <t>Orthopädisches Spital Speising</t>
         </is>
       </c>
-      <c r="R299" t="inlineStr"/>
+      <c r="R299" t="inlineStr">
+        <is>
+          <t>Orthopädisches Spital Speising</t>
+        </is>
+      </c>
       <c r="S299" t="inlineStr">
         <is>
           <t>170</t>
@@ -27177,7 +27617,11 @@
           <t>TREIBACHER Industrie AG</t>
         </is>
       </c>
-      <c r="R300" t="inlineStr"/>
+      <c r="R300" t="inlineStr">
+        <is>
+          <t>TREIBACHER Industrie AG</t>
+        </is>
+      </c>
       <c r="S300" t="inlineStr">
         <is>
           <t>240</t>
@@ -27260,7 +27704,11 @@
           <t>WESTbahn</t>
         </is>
       </c>
-      <c r="R301" t="inlineStr"/>
+      <c r="R301" t="inlineStr">
+        <is>
+          <t>WESTbahn</t>
+        </is>
+      </c>
       <c r="S301" t="inlineStr">
         <is>
           <t>110</t>
@@ -27343,7 +27791,11 @@
           <t>HAIDLMAIR GmbH</t>
         </is>
       </c>
-      <c r="R302" t="inlineStr"/>
+      <c r="R302" t="inlineStr">
+        <is>
+          <t>HAIDLMAIR GmbH</t>
+        </is>
+      </c>
       <c r="S302" t="inlineStr">
         <is>
           <t>77</t>
@@ -27426,7 +27878,11 @@
           <t>Österreichische Beamtenversicherung - ÖBV</t>
         </is>
       </c>
-      <c r="R303" t="inlineStr"/>
+      <c r="R303" t="inlineStr">
+        <is>
+          <t>Österreichische Beamtenversicherung - ÖBV</t>
+        </is>
+      </c>
       <c r="S303" t="inlineStr">
         <is>
           <t>190</t>
@@ -27497,7 +27953,11 @@
           <t>EVG Entwicklungs- und Verwertungsgesellschaft GmbH</t>
         </is>
       </c>
-      <c r="R304" t="inlineStr"/>
+      <c r="R304" t="inlineStr">
+        <is>
+          <t>EVG Entwicklungs- und Verwertungsgesellschaft GmbH</t>
+        </is>
+      </c>
       <c r="S304" t="inlineStr">
         <is>
           <t>85</t>
@@ -27580,7 +28040,11 @@
           <t>Stadt Innsbruck</t>
         </is>
       </c>
-      <c r="R305" t="inlineStr"/>
+      <c r="R305" t="inlineStr">
+        <is>
+          <t>Stadt Innsbruck</t>
+        </is>
+      </c>
       <c r="S305" t="inlineStr">
         <is>
           <t>160</t>
@@ -27663,7 +28127,11 @@
           <t>ENERGIEALLIANZ Austria GmbH</t>
         </is>
       </c>
-      <c r="R306" t="inlineStr"/>
+      <c r="R306" t="inlineStr">
+        <is>
+          <t>ENERGIEALLIANZ Austria GmbH</t>
+        </is>
+      </c>
       <c r="S306" t="inlineStr">
         <is>
           <t>86</t>
@@ -27746,7 +28214,11 @@
           <t>Ankerbrot</t>
         </is>
       </c>
-      <c r="R307" t="inlineStr"/>
+      <c r="R307" t="inlineStr">
+        <is>
+          <t>Ankerbrot</t>
+        </is>
+      </c>
       <c r="S307" t="inlineStr">
         <is>
           <t>130</t>
@@ -27829,7 +28301,11 @@
           <t>ENERGIEALLIANZ Austria GmbH</t>
         </is>
       </c>
-      <c r="R308" t="inlineStr"/>
+      <c r="R308" t="inlineStr">
+        <is>
+          <t>ENERGIEALLIANZ Austria GmbH</t>
+        </is>
+      </c>
       <c r="S308" t="inlineStr">
         <is>
           <t>86</t>
@@ -27904,7 +28380,11 @@
           <t>GIG Karasek GmbH - A Member of Dr. Aichhorn Group</t>
         </is>
       </c>
-      <c r="R309" t="inlineStr"/>
+      <c r="R309" t="inlineStr">
+        <is>
+          <t>GIG Karasek GmbH - A Member of Dr. Aichhorn Group</t>
+        </is>
+      </c>
       <c r="S309" t="inlineStr">
         <is>
           <t>68</t>
@@ -27979,7 +28459,11 @@
           <t>WESTbahn</t>
         </is>
       </c>
-      <c r="R310" t="inlineStr"/>
+      <c r="R310" t="inlineStr">
+        <is>
+          <t>WESTbahn</t>
+        </is>
+      </c>
       <c r="S310" t="inlineStr">
         <is>
           <t>110</t>
@@ -28054,7 +28538,11 @@
           <t>JOANNEUM RESEARCH</t>
         </is>
       </c>
-      <c r="R311" t="inlineStr"/>
+      <c r="R311" t="inlineStr">
+        <is>
+          <t>JOANNEUM RESEARCH</t>
+        </is>
+      </c>
       <c r="S311" t="inlineStr">
         <is>
           <t>390</t>
@@ -28137,7 +28625,11 @@
           <t>Polymer Competence Center Leoben GmbH (PCCL)</t>
         </is>
       </c>
-      <c r="R312" t="inlineStr"/>
+      <c r="R312" t="inlineStr">
+        <is>
+          <t>Polymer Competence Center Leoben GmbH (PCCL)</t>
+        </is>
+      </c>
       <c r="S312" t="inlineStr">
         <is>
           <t>70</t>
@@ -28212,7 +28704,11 @@
           <t>RO-RA Aviation Systems GmbH</t>
         </is>
       </c>
-      <c r="R313" t="inlineStr"/>
+      <c r="R313" t="inlineStr">
+        <is>
+          <t>RO-RA Aviation Systems GmbH</t>
+        </is>
+      </c>
       <c r="S313" t="inlineStr">
         <is>
           <t>79</t>
@@ -28287,7 +28783,11 @@
           <t>Burgenland Energie AG</t>
         </is>
       </c>
-      <c r="R314" t="inlineStr"/>
+      <c r="R314" t="inlineStr">
+        <is>
+          <t>Burgenland Energie AG</t>
+        </is>
+      </c>
       <c r="S314" t="inlineStr">
         <is>
           <t>240</t>
@@ -28370,7 +28870,11 @@
           <t>Messer Austria</t>
         </is>
       </c>
-      <c r="R315" t="inlineStr"/>
+      <c r="R315" t="inlineStr">
+        <is>
+          <t>Messer Austria</t>
+        </is>
+      </c>
       <c r="S315" t="inlineStr">
         <is>
           <t>51</t>
@@ -28453,7 +28957,11 @@
           <t>Logistik Service GmbH (LogServ)</t>
         </is>
       </c>
-      <c r="R316" t="inlineStr"/>
+      <c r="R316" t="inlineStr">
+        <is>
+          <t>Logistik Service GmbH (LogServ)</t>
+        </is>
+      </c>
       <c r="S316" t="inlineStr">
         <is>
           <t>120</t>
@@ -28532,7 +29040,11 @@
           <t>Apomedica Pharmazeutische Produkte GmbH</t>
         </is>
       </c>
-      <c r="R317" t="inlineStr"/>
+      <c r="R317" t="inlineStr">
+        <is>
+          <t>Apomedica Pharmazeutische Produkte GmbH</t>
+        </is>
+      </c>
       <c r="S317" t="inlineStr">
         <is>
           <t>58</t>
@@ -28607,7 +29119,11 @@
           <t>VOGL + CO</t>
         </is>
       </c>
-      <c r="R318" t="inlineStr"/>
+      <c r="R318" t="inlineStr">
+        <is>
+          <t>VOGL + CO</t>
+        </is>
+      </c>
       <c r="S318" t="inlineStr">
         <is>
           <t>60</t>
@@ -28682,7 +29198,11 @@
           <t>Wiener Privatklinik</t>
         </is>
       </c>
-      <c r="R319" t="inlineStr"/>
+      <c r="R319" t="inlineStr">
+        <is>
+          <t>Wiener Privatklinik</t>
+        </is>
+      </c>
       <c r="S319" t="inlineStr">
         <is>
           <t>88</t>
@@ -28757,7 +29277,11 @@
           <t>Winkelbauer</t>
         </is>
       </c>
-      <c r="R320" t="inlineStr"/>
+      <c r="R320" t="inlineStr">
+        <is>
+          <t>Winkelbauer</t>
+        </is>
+      </c>
       <c r="S320" t="inlineStr">
         <is>
           <t>53</t>
@@ -28840,7 +29364,11 @@
           <t>St. Josef Krankenhaus Wien</t>
         </is>
       </c>
-      <c r="R321" t="inlineStr"/>
+      <c r="R321" t="inlineStr">
+        <is>
+          <t>St. Josef Krankenhaus Wien</t>
+        </is>
+      </c>
       <c r="S321" t="inlineStr">
         <is>
           <t>86</t>
@@ -28923,7 +29451,11 @@
           <t>Wirtschaftsagentur Wien</t>
         </is>
       </c>
-      <c r="R322" t="inlineStr"/>
+      <c r="R322" t="inlineStr">
+        <is>
+          <t>Wirtschaftsagentur Wien</t>
+        </is>
+      </c>
       <c r="S322" t="inlineStr">
         <is>
           <t>180</t>
@@ -29002,7 +29534,11 @@
           <t>GMS GOURMET GmbH</t>
         </is>
       </c>
-      <c r="R323" t="inlineStr"/>
+      <c r="R323" t="inlineStr">
+        <is>
+          <t>GMS GOURMET GmbH</t>
+        </is>
+      </c>
       <c r="S323" t="inlineStr">
         <is>
           <t>310</t>
@@ -29086,7 +29622,11 @@
           <t>FHV - Vorarlberg University of Applied Sciences</t>
         </is>
       </c>
-      <c r="R324" t="inlineStr"/>
+      <c r="R324" t="inlineStr">
+        <is>
+          <t>FHV - Vorarlberg University of Applied Sciences</t>
+        </is>
+      </c>
       <c r="S324" t="inlineStr">
         <is>
           <t>420</t>
@@ -29161,7 +29701,11 @@
           <t>EVG Entwicklungs- und Verwertungsgesellschaft GmbH</t>
         </is>
       </c>
-      <c r="R325" t="inlineStr"/>
+      <c r="R325" t="inlineStr">
+        <is>
+          <t>EVG Entwicklungs- und Verwertungsgesellschaft GmbH</t>
+        </is>
+      </c>
       <c r="S325" t="inlineStr">
         <is>
           <t>85</t>
@@ -29244,7 +29788,11 @@
           <t>HAGE Sondermaschinenbau GmbH</t>
         </is>
       </c>
-      <c r="R326" t="inlineStr"/>
+      <c r="R326" t="inlineStr">
+        <is>
+          <t>HAGE Sondermaschinenbau GmbH</t>
+        </is>
+      </c>
       <c r="S326" t="inlineStr">
         <is>
           <t>51</t>
@@ -29327,7 +29875,11 @@
           <t>Wirtschaftskammer Vorarlberg</t>
         </is>
       </c>
-      <c r="R327" t="inlineStr"/>
+      <c r="R327" t="inlineStr">
+        <is>
+          <t>Wirtschaftskammer Vorarlberg</t>
+        </is>
+      </c>
       <c r="S327" t="inlineStr">
         <is>
           <t>110</t>
@@ -29402,7 +29954,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R328" t="inlineStr"/>
+      <c r="R328" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S328" t="inlineStr">
         <is>
           <t>400</t>
@@ -29485,7 +30041,11 @@
           <t>Krankenhaus der Barmherzigen Schwestern Ried</t>
         </is>
       </c>
-      <c r="R329" t="inlineStr"/>
+      <c r="R329" t="inlineStr">
+        <is>
+          <t>Krankenhaus der Barmherzigen Schwestern Ried</t>
+        </is>
+      </c>
       <c r="S329" t="inlineStr">
         <is>
           <t>120</t>
@@ -29568,7 +30128,11 @@
           <t>Prangl GmbH</t>
         </is>
       </c>
-      <c r="R330" t="inlineStr"/>
+      <c r="R330" t="inlineStr">
+        <is>
+          <t>Prangl GmbH</t>
+        </is>
+      </c>
       <c r="S330" t="inlineStr">
         <is>
           <t>80</t>
@@ -29651,7 +30215,11 @@
           <t>Häuser zum Leben</t>
         </is>
       </c>
-      <c r="R331" t="inlineStr"/>
+      <c r="R331" t="inlineStr">
+        <is>
+          <t>Häuser zum Leben</t>
+        </is>
+      </c>
       <c r="S331" t="inlineStr">
         <is>
           <t>420</t>
@@ -29734,7 +30302,11 @@
           <t>Lanserhof Group</t>
         </is>
       </c>
-      <c r="R332" t="inlineStr"/>
+      <c r="R332" t="inlineStr">
+        <is>
+          <t>Lanserhof Group</t>
+        </is>
+      </c>
       <c r="S332" t="inlineStr">
         <is>
           <t>160</t>
@@ -29817,7 +30389,11 @@
           <t>Gesundheits- und Thermenresort Warmbad-Villach</t>
         </is>
       </c>
-      <c r="R333" t="inlineStr"/>
+      <c r="R333" t="inlineStr">
+        <is>
+          <t>Gesundheits- und Thermenresort Warmbad-Villach</t>
+        </is>
+      </c>
       <c r="S333" t="inlineStr">
         <is>
           <t>66</t>
@@ -29900,7 +30476,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R334" t="inlineStr"/>
+      <c r="R334" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S334" t="inlineStr">
         <is>
           <t>400</t>
@@ -29983,7 +30563,11 @@
           <t>EMPL Fahrzeugwerk</t>
         </is>
       </c>
-      <c r="R335" t="inlineStr"/>
+      <c r="R335" t="inlineStr">
+        <is>
+          <t>EMPL Fahrzeugwerk</t>
+        </is>
+      </c>
       <c r="S335" t="inlineStr">
         <is>
           <t>79</t>
@@ -30066,7 +30650,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R336" t="inlineStr"/>
+      <c r="R336" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S336" t="inlineStr">
         <is>
           <t>400</t>
@@ -30141,7 +30729,11 @@
           <t>Pollmann International GmbH</t>
         </is>
       </c>
-      <c r="R337" t="inlineStr"/>
+      <c r="R337" t="inlineStr">
+        <is>
+          <t>Pollmann International GmbH</t>
+        </is>
+      </c>
       <c r="S337" t="inlineStr">
         <is>
           <t>180</t>
@@ -30224,7 +30816,11 @@
           <t>MAN Truck &amp; Bus Vertrieb Österreich GesmbH</t>
         </is>
       </c>
-      <c r="R338" t="inlineStr"/>
+      <c r="R338" t="inlineStr">
+        <is>
+          <t>MAN Truck &amp; Bus Vertrieb Österreich GesmbH</t>
+        </is>
+      </c>
       <c r="S338" t="inlineStr">
         <is>
           <t>130</t>
@@ -30299,7 +30895,11 @@
           <t>NEVEON</t>
         </is>
       </c>
-      <c r="R339" t="inlineStr"/>
+      <c r="R339" t="inlineStr">
+        <is>
+          <t>NEVEON</t>
+        </is>
+      </c>
       <c r="S339" t="inlineStr">
         <is>
           <t>470</t>
@@ -30382,7 +30982,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R340" t="inlineStr"/>
+      <c r="R340" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S340" t="inlineStr">
         <is>
           <t>400</t>
@@ -30457,7 +31061,11 @@
           <t>Energie- und Umweltagentur des Landes NÖ</t>
         </is>
       </c>
-      <c r="R341" t="inlineStr"/>
+      <c r="R341" t="inlineStr">
+        <is>
+          <t>Energie- und Umweltagentur des Landes NÖ</t>
+        </is>
+      </c>
       <c r="S341" t="inlineStr">
         <is>
           <t>56</t>
@@ -30540,7 +31148,11 @@
           <t>FELDER GROUP</t>
         </is>
       </c>
-      <c r="R342" t="inlineStr"/>
+      <c r="R342" t="inlineStr">
+        <is>
+          <t>FELDER GROUP</t>
+        </is>
+      </c>
       <c r="S342" t="inlineStr">
         <is>
           <t>380</t>
@@ -30623,7 +31235,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R343" t="inlineStr"/>
+      <c r="R343" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S343" t="inlineStr">
         <is>
           <t>450</t>
@@ -30706,7 +31322,11 @@
           <t>GIS Aqua Austria GmbH</t>
         </is>
       </c>
-      <c r="R344" t="inlineStr"/>
+      <c r="R344" t="inlineStr">
+        <is>
+          <t>GIS Aqua Austria GmbH</t>
+        </is>
+      </c>
       <c r="S344" t="inlineStr">
         <is>
           <t>57</t>
@@ -30781,7 +31401,11 @@
           <t>Innsbrucker Kommunalbetriebe Aktiengesellschaft</t>
         </is>
       </c>
-      <c r="R345" t="inlineStr"/>
+      <c r="R345" t="inlineStr">
+        <is>
+          <t>Innsbrucker Kommunalbetriebe Aktiengesellschaft</t>
+        </is>
+      </c>
       <c r="S345" t="inlineStr">
         <is>
           <t>230</t>
@@ -30856,7 +31480,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R346" t="inlineStr"/>
+      <c r="R346" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S346" t="inlineStr">
         <is>
           <t>400</t>
@@ -30927,7 +31555,11 @@
           <t>DREHM Pharma GmbH</t>
         </is>
       </c>
-      <c r="R347" t="inlineStr"/>
+      <c r="R347" t="inlineStr">
+        <is>
+          <t>DREHM Pharma GmbH</t>
+        </is>
+      </c>
       <c r="S347" t="inlineStr">
         <is>
           <t>56</t>
@@ -31010,7 +31642,11 @@
           <t>FMW Industries</t>
         </is>
       </c>
-      <c r="R348" t="inlineStr"/>
+      <c r="R348" t="inlineStr">
+        <is>
+          <t>FMW Industries</t>
+        </is>
+      </c>
       <c r="S348" t="inlineStr">
         <is>
           <t>60</t>
@@ -31085,7 +31721,11 @@
           <t>WVP Group</t>
         </is>
       </c>
-      <c r="R349" t="inlineStr"/>
+      <c r="R349" t="inlineStr">
+        <is>
+          <t>WVP Group</t>
+        </is>
+      </c>
       <c r="S349" t="inlineStr">
         <is>
           <t>290</t>
@@ -31160,7 +31800,11 @@
           <t>oekostrom AG</t>
         </is>
       </c>
-      <c r="R350" t="inlineStr"/>
+      <c r="R350" t="inlineStr">
+        <is>
+          <t>oekostrom AG</t>
+        </is>
+      </c>
       <c r="S350" t="inlineStr">
         <is>
           <t>68</t>
@@ -31235,7 +31879,11 @@
           <t>LiSEC Austria GmbH</t>
         </is>
       </c>
-      <c r="R351" t="inlineStr"/>
+      <c r="R351" t="inlineStr">
+        <is>
+          <t>LiSEC Austria GmbH</t>
+        </is>
+      </c>
       <c r="S351" t="inlineStr">
         <is>
           <t>320</t>
@@ -31318,7 +31966,11 @@
           <t>Marcher Fleischwerke Österreich</t>
         </is>
       </c>
-      <c r="R352" t="inlineStr"/>
+      <c r="R352" t="inlineStr">
+        <is>
+          <t>Marcher Fleischwerke Österreich</t>
+        </is>
+      </c>
       <c r="S352" t="inlineStr">
         <is>
           <t>86</t>
@@ -31393,7 +32045,11 @@
           <t>FITINN</t>
         </is>
       </c>
-      <c r="R353" t="inlineStr"/>
+      <c r="R353" t="inlineStr">
+        <is>
+          <t>FITINN</t>
+        </is>
+      </c>
       <c r="S353" t="inlineStr">
         <is>
           <t>200</t>
@@ -31476,7 +32132,11 @@
           <t>Liebscher &amp; Bracht Wien</t>
         </is>
       </c>
-      <c r="R354" t="inlineStr"/>
+      <c r="R354" t="inlineStr">
+        <is>
+          <t>Liebscher &amp; Bracht Wien</t>
+        </is>
+      </c>
       <c r="S354" t="inlineStr">
         <is>
           <t>210</t>
@@ -31555,7 +32215,11 @@
           <t>Fromagerie Bel Maroc SA</t>
         </is>
       </c>
-      <c r="R355" t="inlineStr"/>
+      <c r="R355" t="inlineStr">
+        <is>
+          <t>Fromagerie Bel Maroc SA</t>
+        </is>
+      </c>
       <c r="S355" t="inlineStr">
         <is>
           <t>210</t>
@@ -31626,7 +32290,11 @@
           <t>Starlim Spritzguss GmbH</t>
         </is>
       </c>
-      <c r="R356" t="inlineStr"/>
+      <c r="R356" t="inlineStr">
+        <is>
+          <t>Starlim Spritzguss GmbH</t>
+        </is>
+      </c>
       <c r="S356" t="inlineStr">
         <is>
           <t>240</t>
@@ -31701,7 +32369,11 @@
           <t>OFI Österreichisches Forschungsinstitut für Chemie und Technik</t>
         </is>
       </c>
-      <c r="R357" t="inlineStr"/>
+      <c r="R357" t="inlineStr">
+        <is>
+          <t>OFI Österreichisches Forschungsinstitut für Chemie und Technik</t>
+        </is>
+      </c>
       <c r="S357" t="inlineStr">
         <is>
           <t>68</t>
@@ -31784,7 +32456,11 @@
           <t>Teach For Austria</t>
         </is>
       </c>
-      <c r="R358" t="inlineStr"/>
+      <c r="R358" t="inlineStr">
+        <is>
+          <t>Teach For Austria</t>
+        </is>
+      </c>
       <c r="S358" t="inlineStr">
         <is>
           <t>160</t>
@@ -31867,7 +32543,11 @@
           <t>Federal Ministry of Labour and Economy</t>
         </is>
       </c>
-      <c r="R359" t="inlineStr"/>
+      <c r="R359" t="inlineStr">
+        <is>
+          <t>Federal Ministry of Labour and Economy</t>
+        </is>
+      </c>
       <c r="S359" t="inlineStr">
         <is>
           <t>480</t>
@@ -31950,7 +32630,11 @@
           <t>Häuser zum Leben</t>
         </is>
       </c>
-      <c r="R360" t="inlineStr"/>
+      <c r="R360" t="inlineStr">
+        <is>
+          <t>Häuser zum Leben</t>
+        </is>
+      </c>
       <c r="S360" t="inlineStr">
         <is>
           <t>420</t>
@@ -32033,7 +32717,11 @@
           <t>Dietzel Univolt</t>
         </is>
       </c>
-      <c r="R361" t="inlineStr"/>
+      <c r="R361" t="inlineStr">
+        <is>
+          <t>Dietzel Univolt</t>
+        </is>
+      </c>
       <c r="S361" t="inlineStr">
         <is>
           <t>73</t>
@@ -32116,7 +32804,11 @@
           <t>Neuroth</t>
         </is>
       </c>
-      <c r="R362" t="inlineStr"/>
+      <c r="R362" t="inlineStr">
+        <is>
+          <t>Neuroth</t>
+        </is>
+      </c>
       <c r="S362" t="inlineStr">
         <is>
           <t>420</t>
@@ -32199,7 +32891,11 @@
           <t>OMNi-BiOTiC® by Institut AllergoSan</t>
         </is>
       </c>
-      <c r="R363" t="inlineStr"/>
+      <c r="R363" t="inlineStr">
+        <is>
+          <t>OMNi-BiOTiC® by Institut AllergoSan</t>
+        </is>
+      </c>
       <c r="S363" t="inlineStr">
         <is>
           <t>230</t>
@@ -32274,7 +32970,11 @@
           <t>Stadt Villach</t>
         </is>
       </c>
-      <c r="R364" t="inlineStr"/>
+      <c r="R364" t="inlineStr">
+        <is>
+          <t>Stadt Villach</t>
+        </is>
+      </c>
       <c r="S364" t="inlineStr">
         <is>
           <t>140</t>
@@ -32357,7 +33057,11 @@
           <t>NEVEON</t>
         </is>
       </c>
-      <c r="R365" t="inlineStr"/>
+      <c r="R365" t="inlineStr">
+        <is>
+          <t>NEVEON</t>
+        </is>
+      </c>
       <c r="S365" t="inlineStr">
         <is>
           <t>470</t>
@@ -32440,7 +33144,11 @@
           <t>Greiner Assistec</t>
         </is>
       </c>
-      <c r="R366" t="inlineStr"/>
+      <c r="R366" t="inlineStr">
+        <is>
+          <t>Greiner Assistec</t>
+        </is>
+      </c>
       <c r="S366" t="inlineStr">
         <is>
           <t>220</t>
@@ -32515,7 +33223,11 @@
           <t>Boxmark Leather</t>
         </is>
       </c>
-      <c r="R367" t="inlineStr"/>
+      <c r="R367" t="inlineStr">
+        <is>
+          <t>Boxmark Leather</t>
+        </is>
+      </c>
       <c r="S367" t="inlineStr">
         <is>
           <t>390</t>
@@ -32598,7 +33310,11 @@
           <t>faigle Kunststoffe GmbH</t>
         </is>
       </c>
-      <c r="R368" t="inlineStr"/>
+      <c r="R368" t="inlineStr">
+        <is>
+          <t>faigle Kunststoffe GmbH</t>
+        </is>
+      </c>
       <c r="S368" t="inlineStr">
         <is>
           <t>64</t>
@@ -32673,7 +33389,11 @@
           <t>Bundesverwaltungsgericht Österreich</t>
         </is>
       </c>
-      <c r="R369" t="inlineStr"/>
+      <c r="R369" t="inlineStr">
+        <is>
+          <t>Bundesverwaltungsgericht Österreich</t>
+        </is>
+      </c>
       <c r="S369" t="inlineStr">
         <is>
           <t>96</t>
@@ -32756,7 +33476,11 @@
           <t>Alba Industries GmbH</t>
         </is>
       </c>
-      <c r="R370" t="inlineStr"/>
+      <c r="R370" t="inlineStr">
+        <is>
+          <t>Alba Industries GmbH</t>
+        </is>
+      </c>
       <c r="S370" t="inlineStr">
         <is>
           <t>51</t>
@@ -32839,7 +33563,11 @@
           <t>Evangelisches Krankenhaus in Wien</t>
         </is>
       </c>
-      <c r="R371" t="inlineStr"/>
+      <c r="R371" t="inlineStr">
+        <is>
+          <t>Evangelisches Krankenhaus in Wien</t>
+        </is>
+      </c>
       <c r="S371" t="inlineStr">
         <is>
           <t>87</t>
@@ -32922,7 +33650,11 @@
           <t>CCE</t>
         </is>
       </c>
-      <c r="R372" t="inlineStr"/>
+      <c r="R372" t="inlineStr">
+        <is>
+          <t>CCE</t>
+        </is>
+      </c>
       <c r="S372" t="inlineStr">
         <is>
           <t>310</t>
@@ -33005,7 +33737,11 @@
           <t>Murexin GmbH</t>
         </is>
       </c>
-      <c r="R373" t="inlineStr"/>
+      <c r="R373" t="inlineStr">
+        <is>
+          <t>Murexin GmbH</t>
+        </is>
+      </c>
       <c r="S373" t="inlineStr">
         <is>
           <t>97</t>
@@ -33088,7 +33824,11 @@
           <t>Marcher Fleischwerke Österreich</t>
         </is>
       </c>
-      <c r="R374" t="inlineStr"/>
+      <c r="R374" t="inlineStr">
+        <is>
+          <t>Marcher Fleischwerke Österreich</t>
+        </is>
+      </c>
       <c r="S374" t="inlineStr">
         <is>
           <t>86</t>
@@ -33171,7 +33911,11 @@
           <t>ELIN Motoren GmbH - A Voith Company</t>
         </is>
       </c>
-      <c r="R375" t="inlineStr"/>
+      <c r="R375" t="inlineStr">
+        <is>
+          <t>ELIN Motoren GmbH - A Voith Company</t>
+        </is>
+      </c>
       <c r="S375" t="inlineStr">
         <is>
           <t>210</t>
@@ -33246,7 +33990,11 @@
           <t>Klinikum Wels-Grieskirchen GmbH</t>
         </is>
       </c>
-      <c r="R376" t="inlineStr"/>
+      <c r="R376" t="inlineStr">
+        <is>
+          <t>Klinikum Wels-Grieskirchen GmbH</t>
+        </is>
+      </c>
       <c r="S376" t="inlineStr">
         <is>
           <t>440</t>
@@ -33317,7 +34065,11 @@
           <t>Erne Fittings GmbH</t>
         </is>
       </c>
-      <c r="R377" t="inlineStr"/>
+      <c r="R377" t="inlineStr">
+        <is>
+          <t>Erne Fittings GmbH</t>
+        </is>
+      </c>
       <c r="S377" t="inlineStr">
         <is>
           <t>110</t>
@@ -33400,7 +34152,11 @@
           <t>Pipelife Austria</t>
         </is>
       </c>
-      <c r="R378" t="inlineStr"/>
+      <c r="R378" t="inlineStr">
+        <is>
+          <t>Pipelife Austria</t>
+        </is>
+      </c>
       <c r="S378" t="inlineStr">
         <is>
           <t>75</t>
@@ -33475,7 +34231,11 @@
           <t>Aspöck Systems</t>
         </is>
       </c>
-      <c r="R379" t="inlineStr"/>
+      <c r="R379" t="inlineStr">
+        <is>
+          <t>Aspöck Systems</t>
+        </is>
+      </c>
       <c r="S379" t="inlineStr">
         <is>
           <t>490</t>
@@ -33554,7 +34314,11 @@
           <t>MOON POWER GmbH</t>
         </is>
       </c>
-      <c r="R380" t="inlineStr"/>
+      <c r="R380" t="inlineStr">
+        <is>
+          <t>MOON POWER GmbH</t>
+        </is>
+      </c>
       <c r="S380" t="inlineStr">
         <is>
           <t>64</t>
@@ -33637,7 +34401,11 @@
           <t>Wolfgang Denzel Auto AG</t>
         </is>
       </c>
-      <c r="R381" t="inlineStr"/>
+      <c r="R381" t="inlineStr">
+        <is>
+          <t>Wolfgang Denzel Auto AG</t>
+        </is>
+      </c>
       <c r="S381" t="inlineStr">
         <is>
           <t>340</t>
@@ -33712,7 +34480,11 @@
           <t>11er Nahrungsmittel GmbH</t>
         </is>
       </c>
-      <c r="R382" t="inlineStr"/>
+      <c r="R382" t="inlineStr">
+        <is>
+          <t>11er Nahrungsmittel GmbH</t>
+        </is>
+      </c>
       <c r="S382" t="inlineStr">
         <is>
           <t>77</t>
@@ -33795,7 +34567,11 @@
           <t>BIOGENA GROUP</t>
         </is>
       </c>
-      <c r="R383" t="inlineStr"/>
+      <c r="R383" t="inlineStr">
+        <is>
+          <t>BIOGENA GROUP</t>
+        </is>
+      </c>
       <c r="S383" t="inlineStr">
         <is>
           <t>220</t>
@@ -33878,7 +34654,11 @@
           <t>Hawle Austria Group</t>
         </is>
       </c>
-      <c r="R384" t="inlineStr"/>
+      <c r="R384" t="inlineStr">
+        <is>
+          <t>Hawle Austria Group</t>
+        </is>
+      </c>
       <c r="S384" t="inlineStr">
         <is>
           <t>500</t>
@@ -33961,7 +34741,11 @@
           <t>HAINZL Industriesysteme GmbH</t>
         </is>
       </c>
-      <c r="R385" t="inlineStr"/>
+      <c r="R385" t="inlineStr">
+        <is>
+          <t>HAINZL Industriesysteme GmbH</t>
+        </is>
+      </c>
       <c r="S385" t="inlineStr">
         <is>
           <t>290</t>
@@ -34036,7 +34820,11 @@
           <t>Alpine Metal Tech Group</t>
         </is>
       </c>
-      <c r="R386" t="inlineStr"/>
+      <c r="R386" t="inlineStr">
+        <is>
+          <t>Alpine Metal Tech Group</t>
+        </is>
+      </c>
       <c r="S386" t="inlineStr">
         <is>
           <t>170</t>
@@ -34111,7 +34899,11 @@
           <t>WINTERSTEIGER Group</t>
         </is>
       </c>
-      <c r="R387" t="inlineStr"/>
+      <c r="R387" t="inlineStr">
+        <is>
+          <t>WINTERSTEIGER Group</t>
+        </is>
+      </c>
       <c r="S387" t="inlineStr">
         <is>
           <t>340</t>
@@ -34187,7 +34979,11 @@
           <t>Kostwein Maschinenbau GmbH</t>
         </is>
       </c>
-      <c r="R388" t="inlineStr"/>
+      <c r="R388" t="inlineStr">
+        <is>
+          <t>Kostwein Maschinenbau GmbH</t>
+        </is>
+      </c>
       <c r="S388" t="inlineStr">
         <is>
           <t>170</t>
@@ -34270,7 +35066,11 @@
           <t>AMST-Systemtechnik GmbH</t>
         </is>
       </c>
-      <c r="R389" t="inlineStr"/>
+      <c r="R389" t="inlineStr">
+        <is>
+          <t>AMST-Systemtechnik GmbH</t>
+        </is>
+      </c>
       <c r="S389" t="inlineStr">
         <is>
           <t>85</t>
@@ -34345,7 +35145,11 @@
           <t>ITS. Implants</t>
         </is>
       </c>
-      <c r="R390" t="inlineStr"/>
+      <c r="R390" t="inlineStr">
+        <is>
+          <t>ITS. Implants</t>
+        </is>
+      </c>
       <c r="S390" t="inlineStr">
         <is>
           <t>160</t>
@@ -34420,7 +35224,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R391" t="inlineStr"/>
+      <c r="R391" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S391" t="inlineStr">
         <is>
           <t>400</t>
@@ -34503,7 +35311,11 @@
           <t>Martin Auer</t>
         </is>
       </c>
-      <c r="R392" t="inlineStr"/>
+      <c r="R392" t="inlineStr">
+        <is>
+          <t>Martin Auer</t>
+        </is>
+      </c>
       <c r="S392" t="inlineStr">
         <is>
           <t>71</t>
@@ -34578,7 +35390,11 @@
           <t>ITS. Implants</t>
         </is>
       </c>
-      <c r="R393" t="inlineStr"/>
+      <c r="R393" t="inlineStr">
+        <is>
+          <t>ITS. Implants</t>
+        </is>
+      </c>
       <c r="S393" t="inlineStr">
         <is>
           <t>160</t>
@@ -34661,7 +35477,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R394" t="inlineStr"/>
+      <c r="R394" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S394" t="inlineStr">
         <is>
           <t>400</t>
@@ -34744,7 +35564,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R395" t="inlineStr"/>
+      <c r="R395" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S395" t="inlineStr">
         <is>
           <t>400</t>
@@ -34815,7 +35639,11 @@
           <t>AUSTRIA JUICE Group</t>
         </is>
       </c>
-      <c r="R396" t="inlineStr"/>
+      <c r="R396" t="inlineStr">
+        <is>
+          <t>AUSTRIA JUICE Group</t>
+        </is>
+      </c>
       <c r="S396" t="inlineStr">
         <is>
           <t>160</t>
@@ -34898,7 +35726,11 @@
           <t>Linde Gas GmbH Österreich</t>
         </is>
       </c>
-      <c r="R397" t="inlineStr"/>
+      <c r="R397" t="inlineStr">
+        <is>
+          <t>Linde Gas GmbH Österreich</t>
+        </is>
+      </c>
       <c r="S397" t="inlineStr">
         <is>
           <t>73</t>
@@ -34973,7 +35805,11 @@
           <t>Ribbon Bio</t>
         </is>
       </c>
-      <c r="R398" t="inlineStr"/>
+      <c r="R398" t="inlineStr">
+        <is>
+          <t>Ribbon Bio</t>
+        </is>
+      </c>
       <c r="S398" t="inlineStr">
         <is>
           <t>53</t>
@@ -35048,7 +35884,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R399" t="inlineStr"/>
+      <c r="R399" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S399" t="inlineStr">
         <is>
           <t>450</t>
@@ -35131,7 +35971,11 @@
           <t>pro medico HandelsGmbH</t>
         </is>
       </c>
-      <c r="R400" t="inlineStr"/>
+      <c r="R400" t="inlineStr">
+        <is>
+          <t>pro medico HandelsGmbH</t>
+        </is>
+      </c>
       <c r="S400" t="inlineStr">
         <is>
           <t>83</t>
@@ -35214,7 +36058,11 @@
           <t>IBS Paper Performance Group</t>
         </is>
       </c>
-      <c r="R401" t="inlineStr"/>
+      <c r="R401" t="inlineStr">
+        <is>
+          <t>IBS Paper Performance Group</t>
+        </is>
+      </c>
       <c r="S401" t="inlineStr">
         <is>
           <t>290</t>
@@ -35289,7 +36137,11 @@
           <t>WINTERSTEIGER Group</t>
         </is>
       </c>
-      <c r="R402" t="inlineStr"/>
+      <c r="R402" t="inlineStr">
+        <is>
+          <t>WINTERSTEIGER Group</t>
+        </is>
+      </c>
       <c r="S402" t="inlineStr">
         <is>
           <t>340</t>
@@ -35364,7 +36216,11 @@
           <t>Kardinal Schwarzenberg Klinikum GmbH</t>
         </is>
       </c>
-      <c r="R403" t="inlineStr"/>
+      <c r="R403" t="inlineStr">
+        <is>
+          <t>Kardinal Schwarzenberg Klinikum GmbH</t>
+        </is>
+      </c>
       <c r="S403" t="inlineStr">
         <is>
           <t>140</t>
@@ -35447,7 +36303,11 @@
           <t>Rupp AG</t>
         </is>
       </c>
-      <c r="R404" t="inlineStr"/>
+      <c r="R404" t="inlineStr">
+        <is>
+          <t>Rupp AG</t>
+        </is>
+      </c>
       <c r="S404" t="inlineStr">
         <is>
           <t>110</t>
@@ -35530,7 +36390,11 @@
           <t>TROX Austria &amp; CEE</t>
         </is>
       </c>
-      <c r="R405" t="inlineStr"/>
+      <c r="R405" t="inlineStr">
+        <is>
+          <t>TROX Austria &amp; CEE</t>
+        </is>
+      </c>
       <c r="S405" t="inlineStr">
         <is>
           <t>51</t>
@@ -35605,7 +36469,11 @@
           <t>AGILOX</t>
         </is>
       </c>
-      <c r="R406" t="inlineStr"/>
+      <c r="R406" t="inlineStr">
+        <is>
+          <t>AGILOX</t>
+        </is>
+      </c>
       <c r="S406" t="inlineStr">
         <is>
           <t>180</t>
@@ -35688,7 +36556,11 @@
           <t>MedAustron</t>
         </is>
       </c>
-      <c r="R407" t="inlineStr"/>
+      <c r="R407" t="inlineStr">
+        <is>
+          <t>MedAustron</t>
+        </is>
+      </c>
       <c r="S407" t="inlineStr">
         <is>
           <t>200</t>
@@ -35759,7 +36631,11 @@
           <t>PremiQaMed Group</t>
         </is>
       </c>
-      <c r="R408" t="inlineStr"/>
+      <c r="R408" t="inlineStr">
+        <is>
+          <t>PremiQaMed Group</t>
+        </is>
+      </c>
       <c r="S408" t="inlineStr">
         <is>
           <t>380</t>
@@ -35842,7 +36718,11 @@
           <t>SMB Gruppe</t>
         </is>
       </c>
-      <c r="R409" t="inlineStr"/>
+      <c r="R409" t="inlineStr">
+        <is>
+          <t>SMB Gruppe</t>
+        </is>
+      </c>
       <c r="S409" t="inlineStr">
         <is>
           <t>79</t>
@@ -35917,7 +36797,11 @@
           <t>oekostrom AG</t>
         </is>
       </c>
-      <c r="R410" t="inlineStr"/>
+      <c r="R410" t="inlineStr">
+        <is>
+          <t>oekostrom AG</t>
+        </is>
+      </c>
       <c r="S410" t="inlineStr">
         <is>
           <t>68</t>
@@ -36000,7 +36884,11 @@
           <t>Mazda Austria GmbH</t>
         </is>
       </c>
-      <c r="R411" t="inlineStr"/>
+      <c r="R411" t="inlineStr">
+        <is>
+          <t>Mazda Austria GmbH</t>
+        </is>
+      </c>
       <c r="S411" t="inlineStr">
         <is>
           <t>60</t>
@@ -36075,7 +36963,11 @@
           <t>Logistik Service GmbH (LogServ)</t>
         </is>
       </c>
-      <c r="R412" t="inlineStr"/>
+      <c r="R412" t="inlineStr">
+        <is>
+          <t>Logistik Service GmbH (LogServ)</t>
+        </is>
+      </c>
       <c r="S412" t="inlineStr">
         <is>
           <t>120</t>
@@ -36150,7 +37042,11 @@
           <t>SMB Gruppe</t>
         </is>
       </c>
-      <c r="R413" t="inlineStr"/>
+      <c r="R413" t="inlineStr">
+        <is>
+          <t>SMB Gruppe</t>
+        </is>
+      </c>
       <c r="S413" t="inlineStr">
         <is>
           <t>79</t>
@@ -36233,7 +37129,11 @@
           <t>hollu Systemhygiene GmbH</t>
         </is>
       </c>
-      <c r="R414" t="inlineStr"/>
+      <c r="R414" t="inlineStr">
+        <is>
+          <t>hollu Systemhygiene GmbH</t>
+        </is>
+      </c>
       <c r="S414" t="inlineStr">
         <is>
           <t>210</t>
@@ -36308,7 +37208,11 @@
           <t>Kwizda Agro</t>
         </is>
       </c>
-      <c r="R415" t="inlineStr"/>
+      <c r="R415" t="inlineStr">
+        <is>
+          <t>Kwizda Agro</t>
+        </is>
+      </c>
       <c r="S415" t="inlineStr">
         <is>
           <t>210</t>
@@ -36391,7 +37295,11 @@
           <t>EMCO Corporation</t>
         </is>
       </c>
-      <c r="R416" t="inlineStr"/>
+      <c r="R416" t="inlineStr">
+        <is>
+          <t>EMCO Corporation</t>
+        </is>
+      </c>
       <c r="S416" t="inlineStr">
         <is>
           <t>360</t>
@@ -36466,7 +37374,11 @@
           <t>Virtual Vehicle Research GmbH</t>
         </is>
       </c>
-      <c r="R417" t="inlineStr"/>
+      <c r="R417" t="inlineStr">
+        <is>
+          <t>Virtual Vehicle Research GmbH</t>
+        </is>
+      </c>
       <c r="S417" t="inlineStr">
         <is>
           <t>250</t>
@@ -36541,7 +37453,11 @@
           <t>Wirtschaftskammer Salzburg</t>
         </is>
       </c>
-      <c r="R418" t="inlineStr"/>
+      <c r="R418" t="inlineStr">
+        <is>
+          <t>Wirtschaftskammer Salzburg</t>
+        </is>
+      </c>
       <c r="S418" t="inlineStr">
         <is>
           <t>130</t>
@@ -36612,7 +37528,11 @@
           <t>JOANNEUM RESEARCH</t>
         </is>
       </c>
-      <c r="R419" t="inlineStr"/>
+      <c r="R419" t="inlineStr">
+        <is>
+          <t>JOANNEUM RESEARCH</t>
+        </is>
+      </c>
       <c r="S419" t="inlineStr">
         <is>
           <t>390</t>
@@ -36691,7 +37611,11 @@
           <t>Bundeskanzleramt Österreich</t>
         </is>
       </c>
-      <c r="R420" t="inlineStr"/>
+      <c r="R420" t="inlineStr">
+        <is>
+          <t>Bundeskanzleramt Österreich</t>
+        </is>
+      </c>
       <c r="S420" t="inlineStr">
         <is>
           <t>260</t>
@@ -36774,7 +37698,11 @@
           <t>Kässbohrer Transport Technik GmbH - Driven by professionals</t>
         </is>
       </c>
-      <c r="R421" t="inlineStr"/>
+      <c r="R421" t="inlineStr">
+        <is>
+          <t>Kässbohrer Transport Technik GmbH - Driven by professionals</t>
+        </is>
+      </c>
       <c r="S421" t="inlineStr">
         <is>
           <t>52</t>
@@ -36849,7 +37777,11 @@
           <t>RUBIG Group</t>
         </is>
       </c>
-      <c r="R422" t="inlineStr"/>
+      <c r="R422" t="inlineStr">
+        <is>
+          <t>RUBIG Group</t>
+        </is>
+      </c>
       <c r="S422" t="inlineStr">
         <is>
           <t>91</t>
@@ -36932,7 +37864,11 @@
           <t>LiSEC Austria GmbH</t>
         </is>
       </c>
-      <c r="R423" t="inlineStr"/>
+      <c r="R423" t="inlineStr">
+        <is>
+          <t>LiSEC Austria GmbH</t>
+        </is>
+      </c>
       <c r="S423" t="inlineStr">
         <is>
           <t>320</t>
@@ -37007,7 +37943,11 @@
           <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
         </is>
       </c>
-      <c r="R424" t="inlineStr"/>
+      <c r="R424" t="inlineStr">
+        <is>
+          <t>Porsche Inter Auto - Österreichs größte Autohandelsgruppe</t>
+        </is>
+      </c>
       <c r="S424" t="inlineStr">
         <is>
           <t>400</t>
@@ -37090,7 +38030,11 @@
           <t>Gabriel-Chemie Group</t>
         </is>
       </c>
-      <c r="R425" t="inlineStr"/>
+      <c r="R425" t="inlineStr">
+        <is>
+          <t>Gabriel-Chemie Group</t>
+        </is>
+      </c>
       <c r="S425" t="inlineStr">
         <is>
           <t>180</t>
@@ -37165,7 +38109,11 @@
           <t>Stadt Villach</t>
         </is>
       </c>
-      <c r="R426" t="inlineStr"/>
+      <c r="R426" t="inlineStr">
+        <is>
+          <t>Stadt Villach</t>
+        </is>
+      </c>
       <c r="S426" t="inlineStr">
         <is>
           <t>140</t>
@@ -37248,7 +38196,11 @@
           <t>KWB GmbH</t>
         </is>
       </c>
-      <c r="R427" t="inlineStr"/>
+      <c r="R427" t="inlineStr">
+        <is>
+          <t>KWB GmbH</t>
+        </is>
+      </c>
       <c r="S427" t="inlineStr">
         <is>
           <t>140</t>
@@ -37331,7 +38283,11 @@
           <t>St. Anna Children's Cancer Research Institute (CCRI)</t>
         </is>
       </c>
-      <c r="R428" t="inlineStr"/>
+      <c r="R428" t="inlineStr">
+        <is>
+          <t>St. Anna Children's Cancer Research Institute (CCRI)</t>
+        </is>
+      </c>
       <c r="S428" t="inlineStr">
         <is>
           <t>170</t>
@@ -37406,7 +38362,11 @@
           <t>Oberösterreichische Versicherung AG</t>
         </is>
       </c>
-      <c r="R429" t="inlineStr"/>
+      <c r="R429" t="inlineStr">
+        <is>
+          <t>Oberösterreichische Versicherung AG</t>
+        </is>
+      </c>
       <c r="S429" t="inlineStr">
         <is>
           <t>200</t>
@@ -37489,7 +38449,11 @@
           <t>PremiQaMed Group</t>
         </is>
       </c>
-      <c r="R430" t="inlineStr"/>
+      <c r="R430" t="inlineStr">
+        <is>
+          <t>PremiQaMed Group</t>
+        </is>
+      </c>
       <c r="S430" t="inlineStr">
         <is>
           <t>380</t>
@@ -37572,7 +38536,11 @@
           <t>PHOENIX CONTACT GmbH</t>
         </is>
       </c>
-      <c r="R431" t="inlineStr"/>
+      <c r="R431" t="inlineStr">
+        <is>
+          <t>PHOENIX CONTACT GmbH</t>
+        </is>
+      </c>
       <c r="S431" t="inlineStr">
         <is>
           <t>82</t>
@@ -37643,7 +38611,11 @@
           <t>Starlim Spritzguss GmbH</t>
         </is>
       </c>
-      <c r="R432" t="inlineStr"/>
+      <c r="R432" t="inlineStr">
+        <is>
+          <t>Starlim Spritzguss GmbH</t>
+        </is>
+      </c>
       <c r="S432" t="inlineStr">
         <is>
           <t>240</t>
@@ -37726,7 +38698,11 @@
           <t>Silicon Austria Labs (SAL)</t>
         </is>
       </c>
-      <c r="R433" t="inlineStr"/>
+      <c r="R433" t="inlineStr">
+        <is>
+          <t>Silicon Austria Labs (SAL)</t>
+        </is>
+      </c>
       <c r="S433" t="inlineStr">
         <is>
           <t>330</t>
@@ -37809,7 +38785,11 @@
           <t>Bundeskanzleramt Österreich</t>
         </is>
       </c>
-      <c r="R434" t="inlineStr"/>
+      <c r="R434" t="inlineStr">
+        <is>
+          <t>Bundeskanzleramt Österreich</t>
+        </is>
+      </c>
       <c r="S434" t="inlineStr">
         <is>
           <t>260</t>
@@ -37884,7 +38864,11 @@
           <t>enspired</t>
         </is>
       </c>
-      <c r="R435" t="inlineStr"/>
+      <c r="R435" t="inlineStr">
+        <is>
+          <t>enspired</t>
+        </is>
+      </c>
       <c r="S435" t="inlineStr">
         <is>
           <t>99</t>
@@ -37967,7 +38951,11 @@
           <t>Bundesministerium für Land- und Forstwirtschaft, Regionen und Wasserwirtschaft</t>
         </is>
       </c>
-      <c r="R436" t="inlineStr"/>
+      <c r="R436" t="inlineStr">
+        <is>
+          <t>Bundesministerium für Land- und Forstwirtschaft, Regionen und Wasserwirtschaft</t>
+        </is>
+      </c>
       <c r="S436" t="inlineStr">
         <is>
           <t>340</t>
@@ -38046,7 +39034,11 @@
           <t>Austrian Federal Chancellery</t>
         </is>
       </c>
-      <c r="R437" t="inlineStr"/>
+      <c r="R437" t="inlineStr">
+        <is>
+          <t>Austrian Federal Chancellery</t>
+        </is>
+      </c>
       <c r="S437" t="inlineStr">
         <is>
           <t>86</t>
@@ -38129,7 +39121,11 @@
           <t>GL Pharma</t>
         </is>
       </c>
-      <c r="R438" t="inlineStr"/>
+      <c r="R438" t="inlineStr">
+        <is>
+          <t>GL Pharma</t>
+        </is>
+      </c>
       <c r="S438" t="inlineStr">
         <is>
           <t>340</t>
@@ -38212,7 +39208,11 @@
           <t>Kremsmueller</t>
         </is>
       </c>
-      <c r="R439" t="inlineStr"/>
+      <c r="R439" t="inlineStr">
+        <is>
+          <t>Kremsmueller</t>
+        </is>
+      </c>
       <c r="S439" t="inlineStr">
         <is>
           <t>310</t>
@@ -38295,7 +39295,11 @@
           <t>Wirtschaftskammer Vorarlberg</t>
         </is>
       </c>
-      <c r="R440" t="inlineStr"/>
+      <c r="R440" t="inlineStr">
+        <is>
+          <t>Wirtschaftskammer Vorarlberg</t>
+        </is>
+      </c>
       <c r="S440" t="inlineStr">
         <is>
           <t>110</t>
@@ -38378,7 +39382,11 @@
           <t>Friedrich Deutsch Metallwerk Ges.m.b.H.</t>
         </is>
       </c>
-      <c r="R441" t="inlineStr"/>
+      <c r="R441" t="inlineStr">
+        <is>
+          <t>Friedrich Deutsch Metallwerk Ges.m.b.H.</t>
+        </is>
+      </c>
       <c r="S441" t="inlineStr">
         <is>
           <t>71</t>
@@ -38453,7 +39461,11 @@
           <t>Virtual Vehicle Research GmbH</t>
         </is>
       </c>
-      <c r="R442" t="inlineStr"/>
+      <c r="R442" t="inlineStr">
+        <is>
+          <t>Virtual Vehicle Research GmbH</t>
+        </is>
+      </c>
       <c r="S442" t="inlineStr">
         <is>
           <t>250</t>
@@ -38528,7 +39540,11 @@
           <t>Mercedes-Benz G GmbH</t>
         </is>
       </c>
-      <c r="R443" t="inlineStr"/>
+      <c r="R443" t="inlineStr">
+        <is>
+          <t>Mercedes-Benz G GmbH</t>
+        </is>
+      </c>
       <c r="S443" t="inlineStr">
         <is>
           <t>360</t>
@@ -38611,7 +39627,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R444" t="inlineStr"/>
+      <c r="R444" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S444" t="inlineStr">
         <is>
           <t>450</t>
@@ -38694,7 +39714,11 @@
           <t>Virtual Vehicle Research GmbH</t>
         </is>
       </c>
-      <c r="R445" t="inlineStr"/>
+      <c r="R445" t="inlineStr">
+        <is>
+          <t>Virtual Vehicle Research GmbH</t>
+        </is>
+      </c>
       <c r="S445" t="inlineStr">
         <is>
           <t>250</t>
@@ -38777,7 +39801,11 @@
           <t>TAG GmbH</t>
         </is>
       </c>
-      <c r="R446" t="inlineStr"/>
+      <c r="R446" t="inlineStr">
+        <is>
+          <t>TAG GmbH</t>
+        </is>
+      </c>
       <c r="S446" t="inlineStr">
         <is>
           <t>110</t>
@@ -38852,7 +39880,11 @@
           <t>Die eww Gruppe</t>
         </is>
       </c>
-      <c r="R447" t="inlineStr"/>
+      <c r="R447" t="inlineStr">
+        <is>
+          <t>Die eww Gruppe</t>
+        </is>
+      </c>
       <c r="S447" t="inlineStr">
         <is>
           <t>280</t>
@@ -38935,7 +39967,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R448" t="inlineStr"/>
+      <c r="R448" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S448" t="inlineStr">
         <is>
           <t>450</t>
@@ -39018,7 +40054,11 @@
           <t>Sozialversicherung der Selbständigen</t>
         </is>
       </c>
-      <c r="R449" t="inlineStr"/>
+      <c r="R449" t="inlineStr">
+        <is>
+          <t>Sozialversicherung der Selbständigen</t>
+        </is>
+      </c>
       <c r="S449" t="inlineStr">
         <is>
           <t>240</t>
@@ -39101,7 +40141,11 @@
           <t>Energie AG OÖ</t>
         </is>
       </c>
-      <c r="R450" t="inlineStr"/>
+      <c r="R450" t="inlineStr">
+        <is>
+          <t>Energie AG OÖ</t>
+        </is>
+      </c>
       <c r="S450" t="inlineStr">
         <is>
           <t>450</t>
@@ -39184,7 +40228,11 @@
           <t>Linde Gas GmbH Österreich</t>
         </is>
       </c>
-      <c r="R451" t="inlineStr"/>
+      <c r="R451" t="inlineStr">
+        <is>
+          <t>Linde Gas GmbH Österreich</t>
+        </is>
+      </c>
       <c r="S451" t="inlineStr">
         <is>
           <t>73</t>
@@ -39267,7 +40315,11 @@
           <t>Richter Pharma AG</t>
         </is>
       </c>
-      <c r="R452" t="inlineStr"/>
+      <c r="R452" t="inlineStr">
+        <is>
+          <t>Richter Pharma AG</t>
+        </is>
+      </c>
       <c r="S452" t="inlineStr">
         <is>
           <t>110</t>
@@ -39350,7 +40402,11 @@
           <t>Hödlmayr International AG</t>
         </is>
       </c>
-      <c r="R453" t="inlineStr"/>
+      <c r="R453" t="inlineStr">
+        <is>
+          <t>Hödlmayr International AG</t>
+        </is>
+      </c>
       <c r="S453" t="inlineStr">
         <is>
           <t>280</t>
@@ -39433,7 +40489,11 @@
           <t>STATISTICS AUSTRIA</t>
         </is>
       </c>
-      <c r="R454" t="inlineStr"/>
+      <c r="R454" t="inlineStr">
+        <is>
+          <t>STATISTICS AUSTRIA</t>
+        </is>
+      </c>
       <c r="S454" t="inlineStr">
         <is>
           <t>330</t>
@@ -39516,7 +40576,11 @@
           <t>HENN Connector Group</t>
         </is>
       </c>
-      <c r="R455" t="inlineStr"/>
+      <c r="R455" t="inlineStr">
+        <is>
+          <t>HENN Connector Group</t>
+        </is>
+      </c>
       <c r="S455" t="inlineStr">
         <is>
           <t>71</t>
@@ -39591,7 +40655,11 @@
           <t>OMNi-BiOTiC® by Institut AllergoSan</t>
         </is>
       </c>
-      <c r="R456" t="inlineStr"/>
+      <c r="R456" t="inlineStr">
+        <is>
+          <t>OMNi-BiOTiC® by Institut AllergoSan</t>
+        </is>
+      </c>
       <c r="S456" t="inlineStr">
         <is>
           <t>230</t>
@@ -39676,7 +40744,11 @@
           <t>Kelly Snacks</t>
         </is>
       </c>
-      <c r="R457" t="inlineStr"/>
+      <c r="R457" t="inlineStr">
+        <is>
+          <t>Kelly Snacks</t>
+        </is>
+      </c>
       <c r="S457" t="inlineStr">
         <is>
           <t>87</t>
@@ -39759,7 +40831,11 @@
           <t>XUND</t>
         </is>
       </c>
-      <c r="R458" t="inlineStr"/>
+      <c r="R458" t="inlineStr">
+        <is>
+          <t>XUND</t>
+        </is>
+      </c>
       <c r="S458" t="inlineStr">
         <is>
           <t>56</t>
@@ -39834,7 +40910,11 @@
           <t>Linsinger Maschinenbau Gmbh</t>
         </is>
       </c>
-      <c r="R459" t="inlineStr"/>
+      <c r="R459" t="inlineStr">
+        <is>
+          <t>Linsinger Maschinenbau Gmbh</t>
+        </is>
+      </c>
       <c r="S459" t="inlineStr">
         <is>
           <t>150</t>
@@ -39917,7 +40997,11 @@
           <t>Wolfgang Denzel Auto AG</t>
         </is>
       </c>
-      <c r="R460" t="inlineStr"/>
+      <c r="R460" t="inlineStr">
+        <is>
+          <t>Wolfgang Denzel Auto AG</t>
+        </is>
+      </c>
       <c r="S460" t="inlineStr">
         <is>
           <t>340</t>
@@ -39992,7 +41076,11 @@
           <t>SKE Engineering GmbH</t>
         </is>
       </c>
-      <c r="R461" t="inlineStr"/>
+      <c r="R461" t="inlineStr">
+        <is>
+          <t>SKE Engineering GmbH</t>
+        </is>
+      </c>
       <c r="S461" t="inlineStr">
         <is>
           <t>98</t>
@@ -40067,7 +41155,11 @@
           <t>Oberösterreichische Versicherung AG</t>
         </is>
       </c>
-      <c r="R462" t="inlineStr"/>
+      <c r="R462" t="inlineStr">
+        <is>
+          <t>Oberösterreichische Versicherung AG</t>
+        </is>
+      </c>
       <c r="S462" t="inlineStr">
         <is>
           <t>200</t>
@@ -40138,7 +41230,11 @@
           <t>PremiQaMed Group</t>
         </is>
       </c>
-      <c r="R463" t="inlineStr"/>
+      <c r="R463" t="inlineStr">
+        <is>
+          <t>PremiQaMed Group</t>
+        </is>
+      </c>
       <c r="S463" t="inlineStr">
         <is>
           <t>380</t>
@@ -40221,7 +41317,11 @@
           <t>Austrian Federal Chancellery</t>
         </is>
       </c>
-      <c r="R464" t="inlineStr"/>
+      <c r="R464" t="inlineStr">
+        <is>
+          <t>Austrian Federal Chancellery</t>
+        </is>
+      </c>
       <c r="S464" t="inlineStr">
         <is>
           <t>86</t>
@@ -40304,7 +41404,11 @@
           <t>Oberösterreichische Versicherung AG</t>
         </is>
       </c>
-      <c r="R465" t="inlineStr"/>
+      <c r="R465" t="inlineStr">
+        <is>
+          <t>Oberösterreichische Versicherung AG</t>
+        </is>
+      </c>
       <c r="S465" t="inlineStr">
         <is>
           <t>200</t>
@@ -40379,7 +41483,11 @@
           <t>oekostrom AG</t>
         </is>
       </c>
-      <c r="R466" t="inlineStr"/>
+      <c r="R466" t="inlineStr">
+        <is>
+          <t>oekostrom AG</t>
+        </is>
+      </c>
       <c r="S466" t="inlineStr">
         <is>
           <t>68</t>
@@ -40462,7 +41570,11 @@
           <t>ESIM Chemicals</t>
         </is>
       </c>
-      <c r="R467" t="inlineStr"/>
+      <c r="R467" t="inlineStr">
+        <is>
+          <t>ESIM Chemicals</t>
+        </is>
+      </c>
       <c r="S467" t="inlineStr">
         <is>
           <t>110</t>
@@ -40545,7 +41657,11 @@
           <t>Gas Connect Austria</t>
         </is>
       </c>
-      <c r="R468" t="inlineStr"/>
+      <c r="R468" t="inlineStr">
+        <is>
+          <t>Gas Connect Austria</t>
+        </is>
+      </c>
       <c r="S468" t="inlineStr">
         <is>
           <t>120</t>
@@ -40628,7 +41744,11 @@
           <t>Binder+Co AG</t>
         </is>
       </c>
-      <c r="R469" t="inlineStr"/>
+      <c r="R469" t="inlineStr">
+        <is>
+          <t>Binder+Co AG</t>
+        </is>
+      </c>
       <c r="S469" t="inlineStr">
         <is>
           <t>120</t>
@@ -40711,7 +41831,11 @@
           <t>LTW Intralogistics GmbH</t>
         </is>
       </c>
-      <c r="R470" t="inlineStr"/>
+      <c r="R470" t="inlineStr">
+        <is>
+          <t>LTW Intralogistics GmbH</t>
+        </is>
+      </c>
       <c r="S470" t="inlineStr">
         <is>
           <t>200</t>
@@ -40794,7 +41918,11 @@
           <t>Doppelmayr Official</t>
         </is>
       </c>
-      <c r="R471" t="inlineStr"/>
+      <c r="R471" t="inlineStr">
+        <is>
+          <t>Doppelmayr Official</t>
+        </is>
+      </c>
       <c r="S471" t="inlineStr">
         <is>
           <t>420</t>
@@ -40877,7 +42005,11 @@
           <t>Dachverband der Sozialversicherungen</t>
         </is>
       </c>
-      <c r="R472" t="inlineStr"/>
+      <c r="R472" t="inlineStr">
+        <is>
+          <t>Dachverband der Sozialversicherungen</t>
+        </is>
+      </c>
       <c r="S472" t="inlineStr">
         <is>
           <t>110</t>
@@ -40960,7 +42092,11 @@
           <t>Sozialversicherung der Selbständigen</t>
         </is>
       </c>
-      <c r="R473" t="inlineStr"/>
+      <c r="R473" t="inlineStr">
+        <is>
+          <t>Sozialversicherung der Selbständigen</t>
+        </is>
+      </c>
       <c r="S473" t="inlineStr">
         <is>
           <t>240</t>
@@ -41035,7 +42171,11 @@
           <t>XUND</t>
         </is>
       </c>
-      <c r="R474" t="inlineStr"/>
+      <c r="R474" t="inlineStr">
+        <is>
+          <t>XUND</t>
+        </is>
+      </c>
       <c r="S474" t="inlineStr">
         <is>
           <t>56</t>
@@ -41118,7 +42258,11 @@
           <t>Wolfgang Denzel Auto AG</t>
         </is>
       </c>
-      <c r="R475" t="inlineStr"/>
+      <c r="R475" t="inlineStr">
+        <is>
+          <t>Wolfgang Denzel Auto AG</t>
+        </is>
+      </c>
       <c r="S475" t="inlineStr">
         <is>
           <t>340</t>
@@ -41193,7 +42337,11 @@
           <t>GL Pharma</t>
         </is>
       </c>
-      <c r="R476" t="inlineStr"/>
+      <c r="R476" t="inlineStr">
+        <is>
+          <t>GL Pharma</t>
+        </is>
+      </c>
       <c r="S476" t="inlineStr">
         <is>
           <t>340</t>
@@ -41276,7 +42424,11 @@
           <t>Oberösterreichische Versicherung AG</t>
         </is>
       </c>
-      <c r="R477" t="inlineStr"/>
+      <c r="R477" t="inlineStr">
+        <is>
+          <t>Oberösterreichische Versicherung AG</t>
+        </is>
+      </c>
       <c r="S477" t="inlineStr">
         <is>
           <t>200</t>
@@ -41359,7 +42511,11 @@
           <t>Bundesministerium für Bildung, Wissenschaft und Forschung</t>
         </is>
       </c>
-      <c r="R478" t="inlineStr"/>
+      <c r="R478" t="inlineStr">
+        <is>
+          <t>Bundesministerium für Bildung, Wissenschaft und Forschung</t>
+        </is>
+      </c>
       <c r="S478" t="inlineStr">
         <is>
           <t>180</t>
@@ -41442,7 +42598,11 @@
           <t>ZIMMER AUSTRIA</t>
         </is>
       </c>
-      <c r="R479" t="inlineStr"/>
+      <c r="R479" t="inlineStr">
+        <is>
+          <t>ZIMMER AUSTRIA</t>
+        </is>
+      </c>
       <c r="S479" t="inlineStr">
         <is>
           <t>79</t>
@@ -41525,7 +42685,11 @@
           <t>SONNENTOR Kräuterhandelsgesellschaft mbH</t>
         </is>
       </c>
-      <c r="R480" t="inlineStr"/>
+      <c r="R480" t="inlineStr">
+        <is>
+          <t>SONNENTOR Kräuterhandelsgesellschaft mbH</t>
+        </is>
+      </c>
       <c r="S480" t="inlineStr">
         <is>
           <t>90</t>
@@ -41600,7 +42764,11 @@
           <t>Virtual Vehicle Research GmbH</t>
         </is>
       </c>
-      <c r="R481" t="inlineStr"/>
+      <c r="R481" t="inlineStr">
+        <is>
+          <t>Virtual Vehicle Research GmbH</t>
+        </is>
+      </c>
       <c r="S481" t="inlineStr">
         <is>
           <t>250</t>
@@ -41683,7 +42851,11 @@
           <t>faigle Kunststoffe GmbH</t>
         </is>
       </c>
-      <c r="R482" t="inlineStr"/>
+      <c r="R482" t="inlineStr">
+        <is>
+          <t>faigle Kunststoffe GmbH</t>
+        </is>
+      </c>
       <c r="S482" t="inlineStr">
         <is>
           <t>64</t>
@@ -41758,7 +42930,11 @@
           <t>Boxmark Leather</t>
         </is>
       </c>
-      <c r="R483" t="inlineStr"/>
+      <c r="R483" t="inlineStr">
+        <is>
+          <t>Boxmark Leather</t>
+        </is>
+      </c>
       <c r="S483" t="inlineStr">
         <is>
           <t>390</t>
@@ -41833,7 +43009,11 @@
           <t>Schiebel</t>
         </is>
       </c>
-      <c r="R484" t="inlineStr"/>
+      <c r="R484" t="inlineStr">
+        <is>
+          <t>Schiebel</t>
+        </is>
+      </c>
       <c r="S484" t="inlineStr">
         <is>
           <t>210</t>
@@ -41908,7 +43088,11 @@
           <t>HENN Connector Group</t>
         </is>
       </c>
-      <c r="R485" t="inlineStr"/>
+      <c r="R485" t="inlineStr">
+        <is>
+          <t>HENN Connector Group</t>
+        </is>
+      </c>
       <c r="S485" t="inlineStr">
         <is>
           <t>71</t>
@@ -41991,7 +43175,11 @@
           <t>A.M.I. Agency for Medical Innovations GmbH</t>
         </is>
       </c>
-      <c r="R486" t="inlineStr"/>
+      <c r="R486" t="inlineStr">
+        <is>
+          <t>A.M.I. Agency for Medical Innovations GmbH</t>
+        </is>
+      </c>
       <c r="S486" t="inlineStr">
         <is>
           <t>59</t>
@@ -42066,7 +43254,11 @@
           <t>MADx – Macro Array Diagnostics GmbH</t>
         </is>
       </c>
-      <c r="R487" t="inlineStr"/>
+      <c r="R487" t="inlineStr">
+        <is>
+          <t>MADx – Macro Array Diagnostics GmbH</t>
+        </is>
+      </c>
       <c r="S487" t="inlineStr">
         <is>
           <t>78</t>
@@ -42149,7 +43341,11 @@
           <t>Mavie Next</t>
         </is>
       </c>
-      <c r="R488" t="inlineStr"/>
+      <c r="R488" t="inlineStr">
+        <is>
+          <t>Mavie Next</t>
+        </is>
+      </c>
       <c r="S488" t="inlineStr">
         <is>
           <t>55</t>
@@ -42224,7 +43420,11 @@
           <t>Hawle Austria Group</t>
         </is>
       </c>
-      <c r="R489" t="inlineStr"/>
+      <c r="R489" t="inlineStr">
+        <is>
+          <t>Hawle Austria Group</t>
+        </is>
+      </c>
       <c r="S489" t="inlineStr">
         <is>
           <t>500</t>
@@ -42303,7 +43503,11 @@
           <t>framag Industrieanlagenbau GmbH</t>
         </is>
       </c>
-      <c r="R490" t="inlineStr"/>
+      <c r="R490" t="inlineStr">
+        <is>
+          <t>framag Industrieanlagenbau GmbH</t>
+        </is>
+      </c>
       <c r="S490" t="inlineStr">
         <is>
           <t>65</t>
@@ -42386,7 +43590,11 @@
           <t>LTW Intralogistics GmbH</t>
         </is>
       </c>
-      <c r="R491" t="inlineStr"/>
+      <c r="R491" t="inlineStr">
+        <is>
+          <t>LTW Intralogistics GmbH</t>
+        </is>
+      </c>
       <c r="S491" t="inlineStr">
         <is>
           <t>200</t>
@@ -42461,7 +43669,11 @@
           <t>DREHM Pharma GmbH</t>
         </is>
       </c>
-      <c r="R492" t="inlineStr"/>
+      <c r="R492" t="inlineStr">
+        <is>
+          <t>DREHM Pharma GmbH</t>
+        </is>
+      </c>
       <c r="S492" t="inlineStr">
         <is>
           <t>56</t>
@@ -42544,7 +43756,11 @@
           <t>SKE Engineering GmbH</t>
         </is>
       </c>
-      <c r="R493" t="inlineStr"/>
+      <c r="R493" t="inlineStr">
+        <is>
+          <t>SKE Engineering GmbH</t>
+        </is>
+      </c>
       <c r="S493" t="inlineStr">
         <is>
           <t>98</t>
@@ -42619,7 +43835,11 @@
           <t>Sanochemia Pharmazeutika</t>
         </is>
       </c>
-      <c r="R494" t="inlineStr"/>
+      <c r="R494" t="inlineStr">
+        <is>
+          <t>Sanochemia Pharmazeutika</t>
+        </is>
+      </c>
       <c r="S494" t="inlineStr">
         <is>
           <t>81</t>
@@ -42694,7 +43914,11 @@
           <t>NEVEON</t>
         </is>
       </c>
-      <c r="R495" t="inlineStr"/>
+      <c r="R495" t="inlineStr">
+        <is>
+          <t>NEVEON</t>
+        </is>
+      </c>
       <c r="S495" t="inlineStr">
         <is>
           <t>470</t>
@@ -42769,7 +43993,11 @@
           <t>Bulung Logistics</t>
         </is>
       </c>
-      <c r="R496" t="inlineStr"/>
+      <c r="R496" t="inlineStr">
+        <is>
+          <t>Bulung Logistics</t>
+        </is>
+      </c>
       <c r="S496" t="inlineStr">
         <is>
           <t>63</t>
@@ -42852,7 +44080,11 @@
           <t>Ankerbrot</t>
         </is>
       </c>
-      <c r="R497" t="inlineStr"/>
+      <c r="R497" t="inlineStr">
+        <is>
+          <t>Ankerbrot</t>
+        </is>
+      </c>
       <c r="S497" t="inlineStr">
         <is>
           <t>130</t>
@@ -42935,7 +44167,11 @@
           <t>Fraunhofer Austria</t>
         </is>
       </c>
-      <c r="R498" t="inlineStr"/>
+      <c r="R498" t="inlineStr">
+        <is>
+          <t>Fraunhofer Austria</t>
+        </is>
+      </c>
       <c r="S498" t="inlineStr">
         <is>
           <t>130</t>
@@ -43018,7 +44254,11 @@
           <t>AXIS Flight Training Systems</t>
         </is>
       </c>
-      <c r="R499" t="inlineStr"/>
+      <c r="R499" t="inlineStr">
+        <is>
+          <t>AXIS Flight Training Systems</t>
+        </is>
+      </c>
       <c r="S499" t="inlineStr">
         <is>
           <t>60</t>
@@ -43093,7 +44333,11 @@
           <t>Seibersdorf Labor GmbH</t>
         </is>
       </c>
-      <c r="R500" t="inlineStr"/>
+      <c r="R500" t="inlineStr">
+        <is>
+          <t>Seibersdorf Labor GmbH</t>
+        </is>
+      </c>
       <c r="S500" t="inlineStr">
         <is>
           <t>87</t>
@@ -43176,7 +44420,11 @@
           <t>AGRANA Starch</t>
         </is>
       </c>
-      <c r="R501" t="inlineStr"/>
+      <c r="R501" t="inlineStr">
+        <is>
+          <t>AGRANA Starch</t>
+        </is>
+      </c>
       <c r="S501" t="inlineStr">
         <is>
           <t>140</t>
@@ -43255,7 +44503,11 @@
           <t>EMCO Corporation</t>
         </is>
       </c>
-      <c r="R502" t="inlineStr"/>
+      <c r="R502" t="inlineStr">
+        <is>
+          <t>EMCO Corporation</t>
+        </is>
+      </c>
       <c r="S502" t="inlineStr">
         <is>
           <t>360</t>
@@ -43338,7 +44590,11 @@
           <t>Neuroth</t>
         </is>
       </c>
-      <c r="R503" t="inlineStr"/>
+      <c r="R503" t="inlineStr">
+        <is>
+          <t>Neuroth</t>
+        </is>
+      </c>
       <c r="S503" t="inlineStr">
         <is>
           <t>420</t>
@@ -43421,7 +44677,11 @@
           <t>MADx – Macro Array Diagnostics GmbH</t>
         </is>
       </c>
-      <c r="R504" t="inlineStr"/>
+      <c r="R504" t="inlineStr">
+        <is>
+          <t>MADx – Macro Array Diagnostics GmbH</t>
+        </is>
+      </c>
       <c r="S504" t="inlineStr">
         <is>
           <t>78</t>
@@ -43504,7 +44764,11 @@
           <t>ZIMM Group</t>
         </is>
       </c>
-      <c r="R505" t="inlineStr"/>
+      <c r="R505" t="inlineStr">
+        <is>
+          <t>ZIMM Group</t>
+        </is>
+      </c>
       <c r="S505" t="inlineStr">
         <is>
           <t>67</t>
@@ -43587,7 +44851,11 @@
           <t>Global Hydro Energy</t>
         </is>
       </c>
-      <c r="R506" t="inlineStr"/>
+      <c r="R506" t="inlineStr">
+        <is>
+          <t>Global Hydro Energy</t>
+        </is>
+      </c>
       <c r="S506" t="inlineStr">
         <is>
           <t>230</t>
@@ -43670,7 +44938,11 @@
           <t>Vorarlberger Landeskrankenhäuser</t>
         </is>
       </c>
-      <c r="R507" t="inlineStr"/>
+      <c r="R507" t="inlineStr">
+        <is>
+          <t>Vorarlberger Landeskrankenhäuser</t>
+        </is>
+      </c>
       <c r="S507" t="inlineStr">
         <is>
           <t>380</t>
@@ -43745,7 +45017,11 @@
           <t>Mosdorfer GmbH</t>
         </is>
       </c>
-      <c r="R508" t="inlineStr"/>
+      <c r="R508" t="inlineStr">
+        <is>
+          <t>Mosdorfer GmbH</t>
+        </is>
+      </c>
       <c r="S508" t="inlineStr">
         <is>
           <t>220</t>
@@ -43828,7 +45104,11 @@
           <t>NEVEON</t>
         </is>
       </c>
-      <c r="R509" t="inlineStr"/>
+      <c r="R509" t="inlineStr">
+        <is>
+          <t>NEVEON</t>
+        </is>
+      </c>
       <c r="S509" t="inlineStr">
         <is>
           <t>470</t>
@@ -43911,7 +45191,11 @@
           <t>ENERGIEALLIANZ Austria GmbH</t>
         </is>
       </c>
-      <c r="R510" t="inlineStr"/>
+      <c r="R510" t="inlineStr">
+        <is>
+          <t>ENERGIEALLIANZ Austria GmbH</t>
+        </is>
+      </c>
       <c r="S510" t="inlineStr">
         <is>
           <t>86</t>
@@ -43994,7 +45278,11 @@
           <t>ENcome Energy Performance</t>
         </is>
       </c>
-      <c r="R511" t="inlineStr"/>
+      <c r="R511" t="inlineStr">
+        <is>
+          <t>ENcome Energy Performance</t>
+        </is>
+      </c>
       <c r="S511" t="inlineStr">
         <is>
           <t>85</t>
@@ -44069,7 +45357,11 @@
           <t>Exelliq</t>
         </is>
       </c>
-      <c r="R512" t="inlineStr"/>
+      <c r="R512" t="inlineStr">
+        <is>
+          <t>Exelliq</t>
+        </is>
+      </c>
       <c r="S512" t="inlineStr">
         <is>
           <t>71</t>
@@ -44152,7 +45444,11 @@
           <t>Trotec Laser</t>
         </is>
       </c>
-      <c r="R513" t="inlineStr"/>
+      <c r="R513" t="inlineStr">
+        <is>
+          <t>Trotec Laser</t>
+        </is>
+      </c>
       <c r="S513" t="inlineStr">
         <is>
           <t>420</t>
@@ -44227,7 +45523,11 @@
           <t>AMEX Healthcare</t>
         </is>
       </c>
-      <c r="R514" t="inlineStr"/>
+      <c r="R514" t="inlineStr">
+        <is>
+          <t>AMEX Healthcare</t>
+        </is>
+      </c>
       <c r="S514" t="inlineStr">
         <is>
           <t>300</t>

</xml_diff>